<commit_message>
updated for 13th May
</commit_message>
<xml_diff>
--- a/data/NZ_COVID19_data.xlsx
+++ b/data/NZ_COVID19_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\moh.govt.nz\dfs-userdata\userstate\iholmste\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B16B02-144F-445E-9AF8-ECC6DF867FC0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56115DD1-AB7F-46A4-B4A7-E80DA61DA32D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1392,7 +1392,7 @@
   <dimension ref="A1:I1151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,7 +1416,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43963.375</v>
+        <v>43964.375</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -9384,7 +9384,7 @@
         <v>93</v>
       </c>
       <c r="E354" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F354" s="5"/>
       <c r="G354" s="5"/>
@@ -27457,7 +27457,7 @@
         <v>98</v>
       </c>
       <c r="E1083" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F1083" s="5"/>
       <c r="G1083" s="5"/>
@@ -29306,9 +29306,7 @@
   </sheetPr>
   <dimension ref="A1:I354"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -29331,7 +29329,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43963.375</v>
+        <v>43964.375</v>
       </c>
       <c r="B2" s="1"/>
     </row>

</xml_diff>

<commit_message>
updated for the 16th May
</commit_message>
<xml_diff>
--- a/data/NZ_COVID19_data.xlsx
+++ b/data/NZ_COVID19_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\moh.govt.nz\dfs-userdata\userstate\iholmste\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\moh.govt.nz\dfs-userdata\userstate\djackson\Desktop\New folder (2)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8309A0E-B3FB-4DCF-8090-069F46E78FE3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F62BD0A-22EB-45A2-8E30-A0D9F58BCD86}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1920" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -22,17 +22,23 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Confirmed!$1:$4</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Probable!$1:$4</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8549" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8550" uniqueCount="331">
   <si>
     <t>BEKA76</t>
   </si>
@@ -1400,9 +1406,7 @@
   </sheetPr>
   <dimension ref="A1:I1152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1425,7 +1429,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43966.375</v>
+        <v>43967.375</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -4247,9 +4251,7 @@
       <c r="G128" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="H128" s="6">
-        <v>43893</v>
-      </c>
+      <c r="H128" s="6"/>
       <c r="I128" s="6">
         <v>43921</v>
       </c>
@@ -12192,9 +12194,7 @@
       <c r="H470" s="6">
         <v>43907</v>
       </c>
-      <c r="I470" s="6">
-        <v>43938</v>
-      </c>
+      <c r="I470" s="6"/>
     </row>
     <row r="471" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A471" s="5" t="s">
@@ -18089,7 +18089,9 @@
       <c r="E718" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F718" s="5"/>
+      <c r="F718" s="5" t="s">
+        <v>128</v>
+      </c>
       <c r="G718" s="5"/>
       <c r="H718" s="6"/>
       <c r="I718" s="6">
@@ -29342,7 +29344,7 @@
   <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
   </mergeCells>
-  <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="43" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
@@ -29354,7 +29356,7 @@
   </sheetPr>
   <dimension ref="A1:I354"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -29377,7 +29379,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43966.375</v>
+        <v>43967.375</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -37126,7 +37128,7 @@
   <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
   </mergeCells>
-  <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="43" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated for the 18th May
</commit_message>
<xml_diff>
--- a/data/NZ_COVID19_data.xlsx
+++ b/data/NZ_COVID19_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\moh.govt.nz\dfs-userdata\userstate\djackson\Desktop\New folder (2)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\moh.govt.nz\dfs-userdata\userstate\iholmste\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6C8F1D-7D40-4783-BEB9-AA3A8630A5C9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BCEB7A6-186C-4CC6-B441-E1D928E25351}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1920" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -22,16 +22,10 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Confirmed!$1:$4</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Probable!$1:$4</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1409,7 +1403,9 @@
   </sheetPr>
   <dimension ref="A1:I1153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="H129" sqref="H129"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1432,7 +1428,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43968.375</v>
+        <v>43969.375</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -29403,7 +29399,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43968.375</v>
+        <v>43969.375</v>
       </c>
       <c r="B2" s="1"/>
     </row>

</xml_diff>

<commit_message>
updated for May 20th
</commit_message>
<xml_diff>
--- a/data/NZ_COVID19_data.xlsx
+++ b/data/NZ_COVID19_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\moh.govt.nz\dfs-userdata\userstate\iholmste\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\moh.govt.nz\dfs-userdata\userstate\crawson\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6115AC-0F2E-4A01-855A-627238D26A5E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E9CA1EF-D46C-4ED7-9377-C699A33468C0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8583" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8584" uniqueCount="334">
   <si>
     <t>BEKA76</t>
   </si>
@@ -1410,7 +1410,7 @@
   <dimension ref="A1:I1157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="I475" sqref="I475"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
-        <v>43970.375</v>
+        <v>43971.375</v>
       </c>
       <c r="B2" s="6"/>
     </row>
@@ -18529,9 +18529,11 @@
       <c r="A735" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B735" s="4"/>
+      <c r="B735" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="C735" s="4" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D735" s="4" t="s">
         <v>95</v>
@@ -18540,16 +18542,16 @@
         <v>116</v>
       </c>
       <c r="F735" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G735" s="4" t="s">
-        <v>246</v>
+        <v>174</v>
       </c>
       <c r="H735" s="5">
-        <v>43910</v>
+        <v>43915</v>
       </c>
       <c r="I735" s="5">
-        <v>43912</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="736" spans="1:9" x14ac:dyDescent="0.25">
@@ -18560,7 +18562,7 @@
         <v>83</v>
       </c>
       <c r="C736" s="4" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D736" s="4" t="s">
         <v>95</v>
@@ -18569,16 +18571,16 @@
         <v>116</v>
       </c>
       <c r="F736" s="4" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="G736" s="4" t="s">
-        <v>174</v>
+        <v>246</v>
       </c>
       <c r="H736" s="5">
-        <v>43915</v>
+        <v>43910</v>
       </c>
       <c r="I736" s="5">
-        <v>43915</v>
+        <v>43912</v>
       </c>
     </row>
     <row r="737" spans="1:9" x14ac:dyDescent="0.25">
@@ -29519,7 +29521,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
-        <v>43970.375</v>
+        <v>43971.375</v>
       </c>
       <c r="B2" s="6"/>
     </row>
@@ -30264,10 +30266,10 @@
         <v>41</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>100</v>
@@ -30285,13 +30287,13 @@
         <v>41</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>115</v>
@@ -30312,7 +30314,7 @@
         <v>87</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>115</v>

</xml_diff>

<commit_message>
updated for the 23rd May
</commit_message>
<xml_diff>
--- a/data/NZ_COVID19_data.xlsx
+++ b/data/NZ_COVID19_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\moh.govt.nz\dfs-userdata\userstate\iholmste\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\moh.govt.nz\dfs-userdata\userstate\arountre\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BBA9D04-3142-44B2-AB4A-26BD0DC79F99}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E3A7A4-01E9-4F0F-899F-A4A5B404FE8C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8591" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8590" uniqueCount="333">
   <si>
     <t>BEKA76</t>
   </si>
@@ -868,9 +868,6 @@
     <t>MH133</t>
   </si>
   <si>
-    <t>WGN-AKL</t>
-  </si>
-  <si>
     <t>MH145</t>
   </si>
   <si>
@@ -1409,8 +1406,8 @@
   </sheetPr>
   <dimension ref="A1:I1158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A442" workbookViewId="0">
-      <selection activeCell="I476" sqref="I476"/>
+    <sheetView tabSelected="1" topLeftCell="A973" workbookViewId="0">
+      <selection activeCell="G861" sqref="G861"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,7 +1431,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43973.375</v>
+        <v>43974.375</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -1902,7 +1899,7 @@
         <v>121</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="6">
@@ -4412,7 +4409,9 @@
       <c r="G134" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="H134" s="6"/>
+      <c r="H134" s="6">
+        <v>43920</v>
+      </c>
       <c r="I134" s="6">
         <v>43921</v>
       </c>
@@ -12359,7 +12358,9 @@
       <c r="H476" s="6">
         <v>43907</v>
       </c>
-      <c r="I476" s="6"/>
+      <c r="I476" s="6">
+        <v>43907</v>
+      </c>
     </row>
     <row r="477" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A477" s="5" t="s">
@@ -21722,9 +21723,7 @@
       <c r="F861" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="G861" s="5" t="s">
-        <v>278</v>
-      </c>
+      <c r="G861" s="5"/>
       <c r="H861" s="6"/>
       <c r="I861" s="6">
         <v>43909</v>
@@ -21996,7 +21995,7 @@
         <v>147</v>
       </c>
       <c r="G872" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H872" s="6">
         <v>43905</v>
@@ -22260,7 +22259,7 @@
         <v>120</v>
       </c>
       <c r="G882" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H882" s="6">
         <v>43911</v>
@@ -22289,7 +22288,7 @@
         <v>126</v>
       </c>
       <c r="G883" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H883" s="6">
         <v>43914</v>
@@ -22539,7 +22538,7 @@
         <v>148</v>
       </c>
       <c r="G893" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H893" s="6">
         <v>43906</v>
@@ -22568,7 +22567,7 @@
         <v>148</v>
       </c>
       <c r="G894" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H894" s="6">
         <v>43906</v>
@@ -22645,7 +22644,7 @@
         <v>127</v>
       </c>
       <c r="G897" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H897" s="6">
         <v>43909</v>
@@ -22878,7 +22877,7 @@
         <v>127</v>
       </c>
       <c r="G906" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H906" s="6">
         <v>43909</v>
@@ -22949,7 +22948,7 @@
         <v>150</v>
       </c>
       <c r="G909" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H909" s="6"/>
       <c r="I909" s="6">
@@ -22976,7 +22975,7 @@
         <v>150</v>
       </c>
       <c r="G910" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H910" s="6">
         <v>43909</v>
@@ -23003,7 +23002,7 @@
       </c>
       <c r="F911" s="5"/>
       <c r="G911" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H911" s="6">
         <v>43909</v>
@@ -23285,7 +23284,7 @@
         <v>120</v>
       </c>
       <c r="G923" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H923" s="6">
         <v>43912</v>
@@ -23402,7 +23401,7 @@
         <v>122</v>
       </c>
       <c r="G928" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H928" s="6">
         <v>43901</v>
@@ -23533,7 +23532,7 @@
         <v>120</v>
       </c>
       <c r="G933" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H933" s="6">
         <v>43912</v>
@@ -23662,7 +23661,7 @@
         <v>145</v>
       </c>
       <c r="G938" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H938" s="6">
         <v>43905</v>
@@ -23741,7 +23740,7 @@
         <v>128</v>
       </c>
       <c r="G941" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H941" s="6">
         <v>43903</v>
@@ -23770,7 +23769,7 @@
         <v>120</v>
       </c>
       <c r="G942" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H942" s="6">
         <v>43909</v>
@@ -23857,7 +23856,7 @@
         <v>119</v>
       </c>
       <c r="G945" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H945" s="6">
         <v>43911</v>
@@ -24036,7 +24035,7 @@
         <v>118</v>
       </c>
       <c r="G952" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H952" s="6">
         <v>43910</v>
@@ -24065,7 +24064,7 @@
         <v>141</v>
       </c>
       <c r="G953" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H953" s="6">
         <v>43910</v>
@@ -24256,7 +24255,7 @@
         <v>119</v>
       </c>
       <c r="G960" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H960" s="6">
         <v>43910</v>
@@ -24306,7 +24305,7 @@
         <v>119</v>
       </c>
       <c r="G962" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H962" s="6">
         <v>43910</v>
@@ -24364,7 +24363,7 @@
         <v>120</v>
       </c>
       <c r="G964" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H964" s="6">
         <v>43910</v>
@@ -24393,7 +24392,7 @@
         <v>127</v>
       </c>
       <c r="G965" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H965" s="6">
         <v>43908</v>
@@ -24422,7 +24421,7 @@
         <v>119</v>
       </c>
       <c r="G966" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H966" s="6">
         <v>43910</v>
@@ -24451,7 +24450,7 @@
         <v>119</v>
       </c>
       <c r="G967" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H967" s="6">
         <v>43910</v>
@@ -24644,7 +24643,7 @@
         <v>120</v>
       </c>
       <c r="G974" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H974" s="6"/>
       <c r="I974" s="6">
@@ -24692,7 +24691,7 @@
         <v>132</v>
       </c>
       <c r="G976" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H976" s="6">
         <v>43906</v>
@@ -24829,7 +24828,7 @@
         <v>123</v>
       </c>
       <c r="G981" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H981" s="6">
         <v>43911</v>
@@ -24904,7 +24903,7 @@
         <v>154</v>
       </c>
       <c r="G984" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H984" s="6">
         <v>43909</v>
@@ -25108,7 +25107,7 @@
         <v>119</v>
       </c>
       <c r="G992" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H992" s="6">
         <v>43907</v>
@@ -25258,7 +25257,7 @@
         <v>145</v>
       </c>
       <c r="G998" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H998" s="6">
         <v>43905</v>
@@ -25308,7 +25307,7 @@
         <v>120</v>
       </c>
       <c r="G1000" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H1000" s="6">
         <v>43909</v>
@@ -25366,7 +25365,7 @@
         <v>147</v>
       </c>
       <c r="G1002" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H1002" s="6">
         <v>43905</v>
@@ -25424,7 +25423,7 @@
         <v>131</v>
       </c>
       <c r="G1004" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H1004" s="6">
         <v>43911</v>
@@ -25551,7 +25550,7 @@
         <v>131</v>
       </c>
       <c r="G1009" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H1009" s="6">
         <v>43909</v>
@@ -25609,7 +25608,7 @@
         <v>119</v>
       </c>
       <c r="G1011" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H1011" s="6">
         <v>43909</v>
@@ -25694,7 +25693,7 @@
         <v>119</v>
       </c>
       <c r="G1014" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H1014" s="6">
         <v>43909</v>
@@ -25808,7 +25807,7 @@
         <v>120</v>
       </c>
       <c r="G1018" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H1018" s="6">
         <v>43907</v>
@@ -25837,7 +25836,7 @@
         <v>120</v>
       </c>
       <c r="G1019" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H1019" s="6">
         <v>43903</v>
@@ -25895,7 +25894,7 @@
         <v>127</v>
       </c>
       <c r="G1021" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H1021" s="6">
         <v>43907</v>
@@ -25945,7 +25944,7 @@
         <v>120</v>
       </c>
       <c r="G1023" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H1023" s="6">
         <v>43908</v>
@@ -26091,7 +26090,7 @@
         <v>125</v>
       </c>
       <c r="G1029" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H1029" s="6">
         <v>43909</v>
@@ -26484,7 +26483,7 @@
         <v>131</v>
       </c>
       <c r="G1044" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H1044" s="6">
         <v>43907</v>
@@ -26613,7 +26612,7 @@
         <v>119</v>
       </c>
       <c r="G1049" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H1049" s="6">
         <v>43906</v>
@@ -26825,7 +26824,7 @@
         <v>119</v>
       </c>
       <c r="G1057" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H1057" s="6">
         <v>43906</v>
@@ -26881,7 +26880,7 @@
       </c>
       <c r="F1059" s="5"/>
       <c r="G1059" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H1059" s="6">
         <v>43898</v>
@@ -26929,7 +26928,7 @@
         <v>120</v>
       </c>
       <c r="G1061" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H1061" s="6"/>
       <c r="I1061" s="6">
@@ -26956,7 +26955,7 @@
         <v>146</v>
       </c>
       <c r="G1062" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H1062" s="6">
         <v>43910</v>
@@ -26985,7 +26984,7 @@
         <v>120</v>
       </c>
       <c r="G1063" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H1063" s="6">
         <v>43908</v>
@@ -27014,7 +27013,7 @@
         <v>120</v>
       </c>
       <c r="G1064" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H1064" s="6"/>
       <c r="I1064" s="6">
@@ -27041,7 +27040,7 @@
         <v>120</v>
       </c>
       <c r="G1065" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H1065" s="6">
         <v>43905</v>
@@ -27303,7 +27302,7 @@
       </c>
       <c r="F1075" s="5"/>
       <c r="G1075" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H1075" s="6">
         <v>43907</v>
@@ -27328,7 +27327,7 @@
       </c>
       <c r="F1076" s="5"/>
       <c r="G1076" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H1076" s="6">
         <v>43905</v>
@@ -27480,7 +27479,7 @@
         <v>146</v>
       </c>
       <c r="G1082" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H1082" s="6">
         <v>43908</v>
@@ -27697,7 +27696,9 @@
         <v>120</v>
       </c>
       <c r="G1091" s="5"/>
-      <c r="H1091" s="6"/>
+      <c r="H1091" s="6">
+        <v>43898</v>
+      </c>
       <c r="I1091" s="6">
         <v>43898</v>
       </c>
@@ -27851,7 +27852,7 @@
         <v>123</v>
       </c>
       <c r="G1097" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H1097" s="6">
         <v>43907</v>
@@ -27928,7 +27929,7 @@
       </c>
       <c r="F1100" s="5"/>
       <c r="G1100" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H1100" s="6">
         <v>43905</v>
@@ -27984,7 +27985,7 @@
         <v>123</v>
       </c>
       <c r="G1102" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H1102" s="6">
         <v>43907</v>
@@ -28042,7 +28043,7 @@
         <v>119</v>
       </c>
       <c r="G1104" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H1104" s="6">
         <v>43906</v>
@@ -28393,7 +28394,7 @@
         <v>120</v>
       </c>
       <c r="G1117" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H1117" s="6">
         <v>43904</v>
@@ -28422,7 +28423,7 @@
         <v>119</v>
       </c>
       <c r="G1118" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H1118" s="6"/>
       <c r="I1118" s="6">
@@ -28497,7 +28498,7 @@
       </c>
       <c r="F1121" s="5"/>
       <c r="G1121" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H1121" s="6">
         <v>43903</v>
@@ -28655,7 +28656,7 @@
       </c>
       <c r="F1127" s="5"/>
       <c r="G1127" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H1127" s="6">
         <v>43894</v>
@@ -28788,7 +28789,7 @@
         <v>120</v>
       </c>
       <c r="G1132" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H1132" s="6">
         <v>43905</v>
@@ -28871,7 +28872,7 @@
         <v>123</v>
       </c>
       <c r="G1135" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H1135" s="6">
         <v>43903</v>
@@ -28958,7 +28959,7 @@
         <v>125</v>
       </c>
       <c r="G1138" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H1138" s="6">
         <v>43906</v>
@@ -29207,7 +29208,7 @@
         <v>132</v>
       </c>
       <c r="G1147" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H1147" s="6">
         <v>43905</v>
@@ -29236,7 +29237,7 @@
         <v>120</v>
       </c>
       <c r="G1148" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H1148" s="6">
         <v>43898</v>
@@ -29315,7 +29316,7 @@
         <v>120</v>
       </c>
       <c r="G1151" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H1151" s="6">
         <v>43903</v>
@@ -29440,7 +29441,7 @@
         <v>131</v>
       </c>
       <c r="G1156" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H1156" s="6">
         <v>43886</v>
@@ -29469,7 +29470,7 @@
         <v>131</v>
       </c>
       <c r="G1157" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H1157" s="6">
         <v>43886</v>
@@ -29546,7 +29547,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43973.375</v>
+        <v>43974.375</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -36256,7 +36257,7 @@
         <v>120</v>
       </c>
       <c r="G310" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H310" s="6">
         <v>43909</v>

</xml_diff>

<commit_message>
updated for the 26th May
</commit_message>
<xml_diff>
--- a/data/NZ_COVID19_data.xlsx
+++ b/data/NZ_COVID19_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\moh.govt.nz\dfs-userdata\userstate\iholmste\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A12A26AD-AE72-401E-B5EB-A0E33A449064}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70BFC692-1A44-4D82-B71A-7F92E9748E87}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8586" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8587" uniqueCount="331">
   <si>
     <t>BEKA76</t>
   </si>
@@ -1400,8 +1400,8 @@
   </sheetPr>
   <dimension ref="A1:I1158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A290" workbookViewId="0">
-      <selection activeCell="G861" sqref="G861"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,7 +1425,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43976.375</v>
+        <v>43977.375</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -2835,7 +2835,9 @@
         <v>124</v>
       </c>
       <c r="G66" s="5"/>
-      <c r="H66" s="6"/>
+      <c r="H66" s="6">
+        <v>43902</v>
+      </c>
       <c r="I66" s="6">
         <v>43933</v>
       </c>
@@ -12868,8 +12870,12 @@
         <v>115</v>
       </c>
       <c r="F498" s="5"/>
-      <c r="G498" s="5"/>
-      <c r="H498" s="6"/>
+      <c r="G498" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="H498" s="6">
+        <v>43909</v>
+      </c>
       <c r="I498" s="6"/>
     </row>
     <row r="499" spans="1:9" x14ac:dyDescent="0.25">
@@ -29531,7 +29537,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43976.375</v>
+        <v>43977.375</v>
       </c>
       <c r="B2" s="1"/>
     </row>

</xml_diff>

<commit_message>
updated for the 28th May
</commit_message>
<xml_diff>
--- a/data/NZ_COVID19_data.xlsx
+++ b/data/NZ_COVID19_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\moh.govt.nz\dfs-userdata\userstate\iholmste\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70BFC692-1A44-4D82-B71A-7F92E9748E87}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{21D0398B-7686-413F-AF1A-5E925A9F2826}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8587" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8588" uniqueCount="332">
   <si>
     <t>BEKA76</t>
   </si>
@@ -548,6 +548,9 @@
   </si>
   <si>
     <t>NZ523</t>
+  </si>
+  <si>
+    <t>NZ1919</t>
   </si>
   <si>
     <t>NZ23</t>
@@ -1400,8 +1403,8 @@
   </sheetPr>
   <dimension ref="A1:I1158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+    <sheetView tabSelected="1" topLeftCell="A452" workbookViewId="0">
+      <selection activeCell="I476" sqref="I476"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,7 +1428,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43977.375</v>
+        <v>43979.375</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -1893,7 +1896,7 @@
         <v>121</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="6">
@@ -4908,7 +4911,9 @@
       <c r="F156" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="G156" s="5"/>
+      <c r="G156" s="5" t="s">
+        <v>172</v>
+      </c>
       <c r="H156" s="6"/>
       <c r="I156" s="6">
         <v>43918</v>
@@ -5097,7 +5102,7 @@
         <v>126</v>
       </c>
       <c r="G164" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H164" s="6">
         <v>43910</v>
@@ -5189,7 +5194,7 @@
         <v>126</v>
       </c>
       <c r="G168" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H168" s="6">
         <v>43913</v>
@@ -5545,7 +5550,7 @@
         <v>120</v>
       </c>
       <c r="G184" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H184" s="6">
         <v>43918</v>
@@ -5771,7 +5776,7 @@
         <v>126</v>
       </c>
       <c r="G194" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H194" s="6"/>
       <c r="I194" s="6">
@@ -5796,7 +5801,7 @@
       </c>
       <c r="F195" s="5"/>
       <c r="G195" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H195" s="6">
         <v>43916</v>
@@ -5886,7 +5891,7 @@
         <v>123</v>
       </c>
       <c r="G199" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H199" s="6">
         <v>43918</v>
@@ -5934,7 +5939,7 @@
       </c>
       <c r="F201" s="5"/>
       <c r="G201" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H201" s="6">
         <v>43913</v>
@@ -6040,7 +6045,7 @@
         <v>119</v>
       </c>
       <c r="G205" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H205" s="6">
         <v>43920</v>
@@ -6090,7 +6095,7 @@
         <v>122</v>
       </c>
       <c r="G207" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H207" s="6">
         <v>43912</v>
@@ -6480,7 +6485,7 @@
         <v>131</v>
       </c>
       <c r="G225" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H225" s="6">
         <v>43909</v>
@@ -6557,7 +6562,7 @@
       </c>
       <c r="F228" s="5"/>
       <c r="G228" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H228" s="6">
         <v>43921</v>
@@ -6745,7 +6750,7 @@
       </c>
       <c r="F236" s="5"/>
       <c r="G236" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H236" s="6">
         <v>43913</v>
@@ -6795,7 +6800,7 @@
       </c>
       <c r="F238" s="5"/>
       <c r="G238" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H238" s="6">
         <v>43913</v>
@@ -6843,7 +6848,7 @@
         <v>127</v>
       </c>
       <c r="G240" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H240" s="6">
         <v>43912</v>
@@ -7166,7 +7171,7 @@
         <v>120</v>
       </c>
       <c r="G255" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H255" s="6">
         <v>43913</v>
@@ -7405,7 +7410,7 @@
         <v>126</v>
       </c>
       <c r="G266" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H266" s="6">
         <v>43910</v>
@@ -7778,7 +7783,7 @@
         <v>132</v>
       </c>
       <c r="G283" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H283" s="6">
         <v>43911</v>
@@ -7853,7 +7858,7 @@
         <v>133</v>
       </c>
       <c r="G286" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H286" s="6">
         <v>43911</v>
@@ -7951,7 +7956,7 @@
       </c>
       <c r="F290" s="5"/>
       <c r="G290" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H290" s="6">
         <v>43911</v>
@@ -7978,7 +7983,7 @@
         <v>120</v>
       </c>
       <c r="G291" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H291" s="6">
         <v>43909</v>
@@ -8181,7 +8186,7 @@
       </c>
       <c r="F300" s="5"/>
       <c r="G300" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H300" s="6">
         <v>43915</v>
@@ -8250,7 +8255,7 @@
         <v>120</v>
       </c>
       <c r="G303" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H303" s="6"/>
       <c r="I303" s="6">
@@ -8461,7 +8466,7 @@
         <v>120</v>
       </c>
       <c r="G312" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H312" s="6">
         <v>43910</v>
@@ -8574,7 +8579,7 @@
         <v>123</v>
       </c>
       <c r="G317" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H317" s="6">
         <v>43918</v>
@@ -8708,7 +8713,7 @@
         <v>126</v>
       </c>
       <c r="G323" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H323" s="6">
         <v>43911</v>
@@ -8821,7 +8826,7 @@
         <v>135</v>
       </c>
       <c r="G328" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H328" s="6">
         <v>43914</v>
@@ -8898,7 +8903,7 @@
       </c>
       <c r="F331" s="5"/>
       <c r="G331" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H331" s="6">
         <v>43909</v>
@@ -8925,7 +8930,7 @@
         <v>131</v>
       </c>
       <c r="G332" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H332" s="6">
         <v>43909</v>
@@ -9063,7 +9068,7 @@
         <v>123</v>
       </c>
       <c r="G338" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H338" s="6"/>
       <c r="I338" s="6">
@@ -9090,7 +9095,7 @@
         <v>123</v>
       </c>
       <c r="G339" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H339" s="6">
         <v>43912</v>
@@ -9266,7 +9271,7 @@
         <v>123</v>
       </c>
       <c r="G347" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H347" s="6">
         <v>43913</v>
@@ -9660,7 +9665,7 @@
         <v>119</v>
       </c>
       <c r="G365" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H365" s="6">
         <v>43918</v>
@@ -9860,7 +9865,7 @@
         <v>123</v>
       </c>
       <c r="G373" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H373" s="6">
         <v>43905</v>
@@ -9973,7 +9978,7 @@
         <v>127</v>
       </c>
       <c r="G378" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H378" s="6">
         <v>43911</v>
@@ -10140,7 +10145,7 @@
         <v>119</v>
       </c>
       <c r="G385" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H385" s="6">
         <v>43914</v>
@@ -10169,7 +10174,7 @@
         <v>119</v>
       </c>
       <c r="G386" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H386" s="6">
         <v>43914</v>
@@ -10198,7 +10203,7 @@
         <v>120</v>
       </c>
       <c r="G387" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H387" s="6">
         <v>43914</v>
@@ -10227,7 +10232,7 @@
         <v>120</v>
       </c>
       <c r="G388" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H388" s="6">
         <v>43914</v>
@@ -10256,7 +10261,7 @@
         <v>132</v>
       </c>
       <c r="G389" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H389" s="6"/>
       <c r="I389" s="6">
@@ -10304,7 +10309,7 @@
         <v>120</v>
       </c>
       <c r="G391" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H391" s="6">
         <v>43908</v>
@@ -10492,7 +10497,7 @@
         <v>123</v>
       </c>
       <c r="G399" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H399" s="6">
         <v>43910</v>
@@ -11015,7 +11020,7 @@
         <v>119</v>
       </c>
       <c r="G422" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H422" s="6">
         <v>43908</v>
@@ -11086,7 +11091,7 @@
         <v>123</v>
       </c>
       <c r="G425" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H425" s="6">
         <v>43913</v>
@@ -11140,7 +11145,7 @@
         <v>119</v>
       </c>
       <c r="G427" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H427" s="6">
         <v>43913</v>
@@ -11283,7 +11288,7 @@
       </c>
       <c r="F432" s="5"/>
       <c r="G432" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H432" s="6">
         <v>43914</v>
@@ -11339,7 +11344,7 @@
         <v>137</v>
       </c>
       <c r="G434" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H434" s="6"/>
       <c r="I434" s="6">
@@ -11502,7 +11507,7 @@
       </c>
       <c r="F441" s="5"/>
       <c r="G441" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H441" s="6">
         <v>43912</v>
@@ -11558,7 +11563,7 @@
         <v>126</v>
       </c>
       <c r="G443" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H443" s="6">
         <v>43915</v>
@@ -11779,7 +11784,7 @@
         <v>120</v>
       </c>
       <c r="G452" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H452" s="6">
         <v>43913</v>
@@ -11892,7 +11897,7 @@
         <v>120</v>
       </c>
       <c r="G457" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H457" s="6">
         <v>43913</v>
@@ -12047,7 +12052,7 @@
         <v>120</v>
       </c>
       <c r="G464" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H464" s="6">
         <v>43913</v>
@@ -12076,7 +12081,7 @@
         <v>131</v>
       </c>
       <c r="G465" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H465" s="6">
         <v>43913</v>
@@ -12166,7 +12171,7 @@
       </c>
       <c r="F469" s="5"/>
       <c r="G469" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H469" s="6">
         <v>43908</v>
@@ -12337,7 +12342,7 @@
         <v>120</v>
       </c>
       <c r="G476" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H476" s="6">
         <v>43907</v>
@@ -12456,7 +12461,7 @@
         <v>119</v>
       </c>
       <c r="G481" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H481" s="6">
         <v>43907</v>
@@ -12506,7 +12511,7 @@
         <v>120</v>
       </c>
       <c r="G483" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H483" s="6">
         <v>43912</v>
@@ -12750,7 +12755,7 @@
       </c>
       <c r="F493" s="5"/>
       <c r="G493" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H493" s="6">
         <v>43918</v>
@@ -12796,7 +12801,7 @@
       </c>
       <c r="F495" s="5"/>
       <c r="G495" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H495" s="6">
         <v>43913</v>
@@ -12823,7 +12828,7 @@
         <v>119</v>
       </c>
       <c r="G496" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H496" s="6">
         <v>43913</v>
@@ -12871,7 +12876,7 @@
       </c>
       <c r="F498" s="5"/>
       <c r="G498" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H498" s="6">
         <v>43909</v>
@@ -12898,7 +12903,7 @@
         <v>131</v>
       </c>
       <c r="G499" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H499" s="6">
         <v>43909</v>
@@ -12927,7 +12932,7 @@
         <v>126</v>
       </c>
       <c r="G500" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H500" s="6">
         <v>43915</v>
@@ -12975,7 +12980,7 @@
       </c>
       <c r="F502" s="5"/>
       <c r="G502" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H502" s="6">
         <v>43915</v>
@@ -13002,7 +13007,7 @@
         <v>122</v>
       </c>
       <c r="G503" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H503" s="6"/>
       <c r="I503" s="6">
@@ -13050,7 +13055,7 @@
         <v>122</v>
       </c>
       <c r="G505" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H505" s="6"/>
       <c r="I505" s="6">
@@ -13098,7 +13103,7 @@
         <v>120</v>
       </c>
       <c r="G507" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H507" s="6">
         <v>43913</v>
@@ -13127,7 +13132,7 @@
         <v>120</v>
       </c>
       <c r="G508" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H508" s="6">
         <v>43913</v>
@@ -13238,7 +13243,7 @@
       </c>
       <c r="F513" s="5"/>
       <c r="G513" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H513" s="6">
         <v>43912</v>
@@ -13288,7 +13293,7 @@
         <v>120</v>
       </c>
       <c r="G515" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H515" s="6">
         <v>43910</v>
@@ -14179,7 +14184,7 @@
       </c>
       <c r="F554" s="5"/>
       <c r="G554" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H554" s="6">
         <v>43910</v>
@@ -14206,7 +14211,7 @@
         <v>123</v>
       </c>
       <c r="G555" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H555" s="6">
         <v>43913</v>
@@ -14260,7 +14265,7 @@
         <v>119</v>
       </c>
       <c r="G557" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H557" s="6"/>
       <c r="I557" s="6">
@@ -14392,7 +14397,7 @@
         <v>119</v>
       </c>
       <c r="G563" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H563" s="6">
         <v>43912</v>
@@ -14465,7 +14470,7 @@
       </c>
       <c r="F566" s="5"/>
       <c r="G566" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H566" s="6">
         <v>43905</v>
@@ -14555,7 +14560,7 @@
         <v>128</v>
       </c>
       <c r="G570" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H570" s="6"/>
       <c r="I570" s="6">
@@ -14582,7 +14587,7 @@
         <v>120</v>
       </c>
       <c r="G571" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H571" s="6">
         <v>43909</v>
@@ -15007,7 +15012,7 @@
         <v>139</v>
       </c>
       <c r="G590" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H590" s="6">
         <v>43907</v>
@@ -15228,7 +15233,7 @@
         <v>120</v>
       </c>
       <c r="G599" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H599" s="6">
         <v>43908</v>
@@ -15257,7 +15262,7 @@
         <v>119</v>
       </c>
       <c r="G600" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H600" s="6">
         <v>43913</v>
@@ -15311,7 +15316,7 @@
         <v>131</v>
       </c>
       <c r="G602" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H602" s="6">
         <v>43909</v>
@@ -15361,7 +15366,7 @@
         <v>120</v>
       </c>
       <c r="G604" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H604" s="6">
         <v>43914</v>
@@ -15390,7 +15395,7 @@
         <v>127</v>
       </c>
       <c r="G605" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H605" s="6">
         <v>43910</v>
@@ -15463,7 +15468,7 @@
         <v>127</v>
       </c>
       <c r="G608" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H608" s="6">
         <v>43912</v>
@@ -15511,7 +15516,7 @@
       </c>
       <c r="F610" s="5"/>
       <c r="G610" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H610" s="6">
         <v>43915</v>
@@ -15580,7 +15585,7 @@
         <v>126</v>
       </c>
       <c r="G613" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H613" s="6">
         <v>43915</v>
@@ -15638,7 +15643,7 @@
         <v>120</v>
       </c>
       <c r="G615" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H615" s="6">
         <v>43909</v>
@@ -15667,7 +15672,7 @@
         <v>132</v>
       </c>
       <c r="G616" s="5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H616" s="6"/>
       <c r="I616" s="6">
@@ -15694,7 +15699,7 @@
         <v>126</v>
       </c>
       <c r="G617" s="5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H617" s="6">
         <v>43913</v>
@@ -16176,7 +16181,7 @@
       </c>
       <c r="F639" s="5"/>
       <c r="G639" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H639" s="6">
         <v>43913</v>
@@ -16442,7 +16447,7 @@
         <v>139</v>
       </c>
       <c r="G651" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H651" s="6">
         <v>43909</v>
@@ -16692,7 +16697,7 @@
         <v>119</v>
       </c>
       <c r="G661" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H661" s="6">
         <v>43908</v>
@@ -16896,7 +16901,7 @@
         <v>119</v>
       </c>
       <c r="G669" s="5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="H669" s="6">
         <v>43905</v>
@@ -17038,7 +17043,7 @@
         <v>120</v>
       </c>
       <c r="G675" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H675" s="6">
         <v>43913</v>
@@ -17067,7 +17072,7 @@
         <v>140</v>
       </c>
       <c r="G676" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H676" s="6">
         <v>43906</v>
@@ -17096,7 +17101,7 @@
         <v>118</v>
       </c>
       <c r="G677" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H677" s="6">
         <v>43905</v>
@@ -17125,7 +17130,7 @@
         <v>123</v>
       </c>
       <c r="G678" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H678" s="6">
         <v>43913</v>
@@ -17154,7 +17159,7 @@
         <v>120</v>
       </c>
       <c r="G679" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H679" s="6">
         <v>43914</v>
@@ -17208,7 +17213,7 @@
         <v>120</v>
       </c>
       <c r="G681" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H681" s="6">
         <v>43914</v>
@@ -17237,7 +17242,7 @@
         <v>127</v>
       </c>
       <c r="G682" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H682" s="6">
         <v>43914</v>
@@ -17266,7 +17271,7 @@
         <v>120</v>
       </c>
       <c r="G683" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H683" s="6">
         <v>43915</v>
@@ -17295,7 +17300,7 @@
         <v>127</v>
       </c>
       <c r="G684" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H684" s="6">
         <v>43912</v>
@@ -17345,7 +17350,7 @@
         <v>127</v>
       </c>
       <c r="G686" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H686" s="6">
         <v>43907</v>
@@ -17537,7 +17542,7 @@
         <v>125</v>
       </c>
       <c r="G694" s="5" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H694" s="6"/>
       <c r="I694" s="6">
@@ -17562,7 +17567,7 @@
       </c>
       <c r="F695" s="5"/>
       <c r="G695" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H695" s="6">
         <v>43908</v>
@@ -17616,7 +17621,7 @@
         <v>119</v>
       </c>
       <c r="G697" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H697" s="6">
         <v>43907</v>
@@ -17712,7 +17717,7 @@
         <v>123</v>
       </c>
       <c r="G701" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H701" s="6">
         <v>43909</v>
@@ -17844,7 +17849,7 @@
       </c>
       <c r="F707" s="5"/>
       <c r="G707" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H707" s="6">
         <v>43906</v>
@@ -17873,7 +17878,7 @@
         <v>123</v>
       </c>
       <c r="G708" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H708" s="6">
         <v>43910</v>
@@ -17923,7 +17928,7 @@
         <v>118</v>
       </c>
       <c r="G710" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H710" s="6">
         <v>43909</v>
@@ -18157,7 +18162,7 @@
         <v>119</v>
       </c>
       <c r="G720" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H720" s="6">
         <v>43908</v>
@@ -18274,7 +18279,7 @@
         <v>119</v>
       </c>
       <c r="G725" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H725" s="6">
         <v>43908</v>
@@ -18374,7 +18379,7 @@
         <v>139</v>
       </c>
       <c r="G729" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H729" s="6">
         <v>43909</v>
@@ -18453,7 +18458,7 @@
         <v>119</v>
       </c>
       <c r="G732" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H732" s="6">
         <v>43908</v>
@@ -18482,7 +18487,7 @@
         <v>127</v>
       </c>
       <c r="G733" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H733" s="6">
         <v>43913</v>
@@ -18509,7 +18514,7 @@
       </c>
       <c r="F734" s="5"/>
       <c r="G734" s="5" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H734" s="6">
         <v>43908</v>
@@ -18534,7 +18539,7 @@
       </c>
       <c r="F735" s="5"/>
       <c r="G735" s="5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H735" s="6">
         <v>43907</v>
@@ -18590,7 +18595,7 @@
         <v>123</v>
       </c>
       <c r="G737" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H737" s="6">
         <v>43910</v>
@@ -18617,7 +18622,7 @@
       </c>
       <c r="F738" s="5"/>
       <c r="G738" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H738" s="6">
         <v>43913</v>
@@ -18644,7 +18649,7 @@
         <v>123</v>
       </c>
       <c r="G739" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="H739" s="6">
         <v>43912</v>
@@ -18671,7 +18676,7 @@
       </c>
       <c r="F740" s="5"/>
       <c r="G740" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H740" s="6">
         <v>43913</v>
@@ -18748,7 +18753,7 @@
         <v>119</v>
       </c>
       <c r="G743" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H743" s="6">
         <v>43912</v>
@@ -18775,7 +18780,7 @@
       </c>
       <c r="F744" s="5"/>
       <c r="G744" s="5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H744" s="6">
         <v>43910</v>
@@ -18823,7 +18828,7 @@
         <v>125</v>
       </c>
       <c r="G746" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H746" s="6">
         <v>43912</v>
@@ -18852,7 +18857,7 @@
         <v>128</v>
       </c>
       <c r="G747" s="5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="H747" s="6">
         <v>43912</v>
@@ -18881,7 +18886,7 @@
         <v>131</v>
       </c>
       <c r="G748" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H748" s="6">
         <v>43910</v>
@@ -18910,7 +18915,7 @@
         <v>131</v>
       </c>
       <c r="G749" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H749" s="6">
         <v>43910</v>
@@ -18939,7 +18944,7 @@
         <v>119</v>
       </c>
       <c r="G750" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H750" s="6">
         <v>43902</v>
@@ -19008,7 +19013,7 @@
       </c>
       <c r="F753" s="5"/>
       <c r="G753" s="5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H753" s="6">
         <v>43909</v>
@@ -19058,7 +19063,7 @@
         <v>119</v>
       </c>
       <c r="G755" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H755" s="6">
         <v>43907</v>
@@ -19129,7 +19134,7 @@
         <v>123</v>
       </c>
       <c r="G758" s="5" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H758" s="6">
         <v>43910</v>
@@ -19368,7 +19373,7 @@
         <v>119</v>
       </c>
       <c r="G769" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H769" s="6"/>
       <c r="I769" s="6">
@@ -19581,7 +19586,7 @@
         <v>123</v>
       </c>
       <c r="G778" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H778" s="6">
         <v>43908</v>
@@ -19610,7 +19615,7 @@
         <v>131</v>
       </c>
       <c r="G779" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H779" s="6">
         <v>43914</v>
@@ -19786,7 +19791,7 @@
         <v>123</v>
       </c>
       <c r="G787" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H787" s="6"/>
       <c r="I787" s="6">
@@ -19882,7 +19887,7 @@
         <v>129</v>
       </c>
       <c r="G791" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H791" s="6">
         <v>43915</v>
@@ -19936,7 +19941,7 @@
         <v>119</v>
       </c>
       <c r="G793" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H793" s="6">
         <v>43912</v>
@@ -19965,7 +19970,7 @@
         <v>119</v>
       </c>
       <c r="G794" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H794" s="6">
         <v>43912</v>
@@ -19994,7 +19999,7 @@
         <v>119</v>
       </c>
       <c r="G795" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H795" s="6">
         <v>43912</v>
@@ -20044,7 +20049,7 @@
         <v>120</v>
       </c>
       <c r="G797" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H797" s="6">
         <v>43914</v>
@@ -20073,7 +20078,7 @@
         <v>120</v>
       </c>
       <c r="G798" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H798" s="6">
         <v>43914</v>
@@ -20102,7 +20107,7 @@
         <v>119</v>
       </c>
       <c r="G799" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H799" s="6">
         <v>43912</v>
@@ -20240,7 +20245,7 @@
         <v>119</v>
       </c>
       <c r="G805" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H805" s="6">
         <v>43908</v>
@@ -20294,7 +20299,7 @@
         <v>125</v>
       </c>
       <c r="G807" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="H807" s="6">
         <v>43913</v>
@@ -20419,7 +20424,7 @@
         <v>120</v>
       </c>
       <c r="G812" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H812" s="6">
         <v>43904</v>
@@ -20448,7 +20453,7 @@
         <v>120</v>
       </c>
       <c r="G813" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H813" s="6">
         <v>43909</v>
@@ -20477,7 +20482,7 @@
         <v>143</v>
       </c>
       <c r="G814" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H814" s="6">
         <v>43908</v>
@@ -20506,7 +20511,7 @@
         <v>126</v>
       </c>
       <c r="G815" s="5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="H815" s="6">
         <v>43908</v>
@@ -20535,7 +20540,7 @@
         <v>119</v>
       </c>
       <c r="G816" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H816" s="6">
         <v>43909</v>
@@ -20635,7 +20640,7 @@
         <v>120</v>
       </c>
       <c r="G820" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="H820" s="6">
         <v>43913</v>
@@ -20664,7 +20669,7 @@
         <v>119</v>
       </c>
       <c r="G821" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H821" s="6">
         <v>43909</v>
@@ -20693,7 +20698,7 @@
         <v>120</v>
       </c>
       <c r="G822" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H822" s="6">
         <v>43914</v>
@@ -20722,7 +20727,7 @@
         <v>119</v>
       </c>
       <c r="G823" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H823" s="6">
         <v>43910</v>
@@ -20801,7 +20806,7 @@
         <v>119</v>
       </c>
       <c r="G826" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H826" s="6">
         <v>43915</v>
@@ -20830,7 +20835,7 @@
         <v>120</v>
       </c>
       <c r="G827" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H827" s="6">
         <v>43910</v>
@@ -20859,7 +20864,7 @@
         <v>120</v>
       </c>
       <c r="G828" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H828" s="6">
         <v>43910</v>
@@ -20909,7 +20914,7 @@
         <v>127</v>
       </c>
       <c r="G830" s="5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H830" s="6">
         <v>43911</v>
@@ -20988,7 +20993,7 @@
         <v>128</v>
       </c>
       <c r="G833" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H833" s="6">
         <v>43909</v>
@@ -21017,7 +21022,7 @@
         <v>125</v>
       </c>
       <c r="G834" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H834" s="6">
         <v>43913</v>
@@ -21119,7 +21124,7 @@
         <v>119</v>
       </c>
       <c r="G838" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="H838" s="6">
         <v>43911</v>
@@ -21148,7 +21153,7 @@
         <v>119</v>
       </c>
       <c r="G839" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H839" s="6"/>
       <c r="I839" s="6">
@@ -21217,7 +21222,7 @@
         <v>146</v>
       </c>
       <c r="G842" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="H842" s="6">
         <v>43906</v>
@@ -21246,7 +21251,7 @@
         <v>119</v>
       </c>
       <c r="G843" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H843" s="6">
         <v>43910</v>
@@ -21296,7 +21301,7 @@
         <v>126</v>
       </c>
       <c r="G845" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H845" s="6">
         <v>43910</v>
@@ -21390,7 +21395,7 @@
       </c>
       <c r="F849" s="5"/>
       <c r="G849" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H849" s="6">
         <v>43910</v>
@@ -21419,7 +21424,7 @@
         <v>130</v>
       </c>
       <c r="G850" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H850" s="6">
         <v>43908</v>
@@ -21448,7 +21453,7 @@
         <v>120</v>
       </c>
       <c r="G851" s="5" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H851" s="6">
         <v>43908</v>
@@ -21556,7 +21561,7 @@
         <v>147</v>
       </c>
       <c r="G855" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H855" s="6">
         <v>43909</v>
@@ -21585,7 +21590,7 @@
         <v>119</v>
       </c>
       <c r="G856" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H856" s="6">
         <v>43913</v>
@@ -21685,7 +21690,7 @@
         <v>120</v>
       </c>
       <c r="G860" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H860" s="6">
         <v>43908</v>
@@ -21739,7 +21744,7 @@
         <v>119</v>
       </c>
       <c r="G862" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H862" s="6">
         <v>43909</v>
@@ -21856,7 +21861,7 @@
         <v>131</v>
       </c>
       <c r="G867" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H867" s="6">
         <v>43907</v>
@@ -21985,7 +21990,7 @@
         <v>147</v>
       </c>
       <c r="G872" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H872" s="6">
         <v>43905</v>
@@ -22014,7 +22019,7 @@
         <v>119</v>
       </c>
       <c r="G873" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H873" s="6">
         <v>43905</v>
@@ -22072,7 +22077,7 @@
         <v>139</v>
       </c>
       <c r="G875" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H875" s="6">
         <v>43909</v>
@@ -22101,7 +22106,7 @@
         <v>120</v>
       </c>
       <c r="G876" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H876" s="6"/>
       <c r="I876" s="6">
@@ -22128,7 +22133,7 @@
         <v>119</v>
       </c>
       <c r="G877" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H877" s="6">
         <v>43910</v>
@@ -22199,7 +22204,7 @@
         <v>120</v>
       </c>
       <c r="G880" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H880" s="6">
         <v>43914</v>
@@ -22249,7 +22254,7 @@
         <v>120</v>
       </c>
       <c r="G882" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="H882" s="6">
         <v>43911</v>
@@ -22278,7 +22283,7 @@
         <v>126</v>
       </c>
       <c r="G883" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="H883" s="6">
         <v>43914</v>
@@ -22307,7 +22312,7 @@
         <v>127</v>
       </c>
       <c r="G884" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H884" s="6">
         <v>43911</v>
@@ -22336,7 +22341,7 @@
         <v>119</v>
       </c>
       <c r="G885" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H885" s="6">
         <v>43909</v>
@@ -22528,7 +22533,7 @@
         <v>148</v>
       </c>
       <c r="G893" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H893" s="6">
         <v>43906</v>
@@ -22557,7 +22562,7 @@
         <v>148</v>
       </c>
       <c r="G894" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H894" s="6">
         <v>43906</v>
@@ -22634,7 +22639,7 @@
         <v>127</v>
       </c>
       <c r="G897" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H897" s="6">
         <v>43909</v>
@@ -22686,7 +22691,7 @@
       </c>
       <c r="F899" s="5"/>
       <c r="G899" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H899" s="6">
         <v>43908</v>
@@ -22867,7 +22872,7 @@
         <v>127</v>
       </c>
       <c r="G906" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="H906" s="6">
         <v>43909</v>
@@ -22938,7 +22943,7 @@
         <v>150</v>
       </c>
       <c r="G909" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="H909" s="6"/>
       <c r="I909" s="6">
@@ -22965,7 +22970,7 @@
         <v>150</v>
       </c>
       <c r="G910" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="H910" s="6">
         <v>43909</v>
@@ -22992,7 +22997,7 @@
       </c>
       <c r="F911" s="5"/>
       <c r="G911" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H911" s="6">
         <v>43909</v>
@@ -23203,7 +23208,7 @@
         <v>131</v>
       </c>
       <c r="G920" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H920" s="6">
         <v>43905</v>
@@ -23274,7 +23279,7 @@
         <v>120</v>
       </c>
       <c r="G923" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H923" s="6">
         <v>43912</v>
@@ -23391,7 +23396,7 @@
         <v>122</v>
       </c>
       <c r="G928" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="H928" s="6">
         <v>43901</v>
@@ -23470,7 +23475,7 @@
         <v>119</v>
       </c>
       <c r="G931" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H931" s="6">
         <v>43907</v>
@@ -23522,7 +23527,7 @@
         <v>120</v>
       </c>
       <c r="G933" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H933" s="6">
         <v>43912</v>
@@ -23580,7 +23585,7 @@
         <v>119</v>
       </c>
       <c r="G935" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H935" s="6">
         <v>43910</v>
@@ -23651,7 +23656,7 @@
         <v>145</v>
       </c>
       <c r="G938" s="5" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H938" s="6">
         <v>43905</v>
@@ -23730,7 +23735,7 @@
         <v>128</v>
       </c>
       <c r="G941" s="5" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H941" s="6">
         <v>43903</v>
@@ -23759,7 +23764,7 @@
         <v>120</v>
       </c>
       <c r="G942" s="5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H942" s="6">
         <v>43909</v>
@@ -23788,7 +23793,7 @@
         <v>119</v>
       </c>
       <c r="G943" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H943" s="6">
         <v>43907</v>
@@ -23846,7 +23851,7 @@
         <v>119</v>
       </c>
       <c r="G945" s="5" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="H945" s="6">
         <v>43911</v>
@@ -23946,7 +23951,7 @@
         <v>119</v>
       </c>
       <c r="G949" s="5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="H949" s="6">
         <v>43905</v>
@@ -23975,7 +23980,7 @@
         <v>119</v>
       </c>
       <c r="G950" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H950" s="6">
         <v>43909</v>
@@ -24025,7 +24030,7 @@
         <v>118</v>
       </c>
       <c r="G952" s="5" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="H952" s="6">
         <v>43910</v>
@@ -24054,7 +24059,7 @@
         <v>141</v>
       </c>
       <c r="G953" s="5" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="H953" s="6">
         <v>43910</v>
@@ -24083,7 +24088,7 @@
         <v>123</v>
       </c>
       <c r="G954" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H954" s="6">
         <v>43909</v>
@@ -24112,7 +24117,7 @@
         <v>123</v>
       </c>
       <c r="G955" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H955" s="6">
         <v>43910</v>
@@ -24141,7 +24146,7 @@
         <v>119</v>
       </c>
       <c r="G956" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H956" s="6">
         <v>43909</v>
@@ -24216,7 +24221,7 @@
         <v>119</v>
       </c>
       <c r="G959" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H959" s="6">
         <v>43907</v>
@@ -24245,7 +24250,7 @@
         <v>119</v>
       </c>
       <c r="G960" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H960" s="6">
         <v>43910</v>
@@ -24295,7 +24300,7 @@
         <v>119</v>
       </c>
       <c r="G962" s="5" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="H962" s="6">
         <v>43910</v>
@@ -24324,7 +24329,7 @@
         <v>120</v>
       </c>
       <c r="G963" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H963" s="6">
         <v>43911</v>
@@ -24353,7 +24358,7 @@
         <v>120</v>
       </c>
       <c r="G964" s="5" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H964" s="6">
         <v>43910</v>
@@ -24382,7 +24387,7 @@
         <v>127</v>
       </c>
       <c r="G965" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="H965" s="6">
         <v>43908</v>
@@ -24411,7 +24416,7 @@
         <v>119</v>
       </c>
       <c r="G966" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H966" s="6">
         <v>43910</v>
@@ -24440,7 +24445,7 @@
         <v>119</v>
       </c>
       <c r="G967" s="5" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="H967" s="6">
         <v>43910</v>
@@ -24633,7 +24638,7 @@
         <v>120</v>
       </c>
       <c r="G974" s="5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H974" s="6"/>
       <c r="I974" s="6">
@@ -24681,7 +24686,7 @@
         <v>132</v>
       </c>
       <c r="G976" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H976" s="6">
         <v>43906</v>
@@ -24760,7 +24765,7 @@
         <v>119</v>
       </c>
       <c r="G979" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H979" s="6">
         <v>43909</v>
@@ -24789,7 +24794,7 @@
         <v>146</v>
       </c>
       <c r="G980" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H980" s="6">
         <v>43913</v>
@@ -24818,7 +24823,7 @@
         <v>123</v>
       </c>
       <c r="G981" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="H981" s="6">
         <v>43911</v>
@@ -24893,7 +24898,7 @@
         <v>154</v>
       </c>
       <c r="G984" s="5" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H984" s="6">
         <v>43909</v>
@@ -24943,7 +24948,7 @@
         <v>123</v>
       </c>
       <c r="G986" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H986" s="6">
         <v>43906</v>
@@ -25018,7 +25023,7 @@
         <v>120</v>
       </c>
       <c r="G989" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H989" s="6">
         <v>43910</v>
@@ -25068,7 +25073,7 @@
         <v>119</v>
       </c>
       <c r="G991" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H991" s="6">
         <v>43906</v>
@@ -25097,7 +25102,7 @@
         <v>119</v>
       </c>
       <c r="G992" s="5" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H992" s="6">
         <v>43907</v>
@@ -25247,7 +25252,7 @@
         <v>145</v>
       </c>
       <c r="G998" s="5" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H998" s="6">
         <v>43905</v>
@@ -25297,7 +25302,7 @@
         <v>120</v>
       </c>
       <c r="G1000" s="5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="H1000" s="6">
         <v>43909</v>
@@ -25326,7 +25331,7 @@
         <v>126</v>
       </c>
       <c r="G1001" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H1001" s="6">
         <v>43909</v>
@@ -25355,7 +25360,7 @@
         <v>147</v>
       </c>
       <c r="G1002" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H1002" s="6">
         <v>43905</v>
@@ -25384,7 +25389,7 @@
         <v>119</v>
       </c>
       <c r="G1003" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H1003" s="6">
         <v>43907</v>
@@ -25413,7 +25418,7 @@
         <v>131</v>
       </c>
       <c r="G1004" s="5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="H1004" s="6">
         <v>43911</v>
@@ -25442,7 +25447,7 @@
         <v>119</v>
       </c>
       <c r="G1005" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H1005" s="6">
         <v>43906</v>
@@ -25540,7 +25545,7 @@
         <v>131</v>
       </c>
       <c r="G1009" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H1009" s="6">
         <v>43909</v>
@@ -25569,7 +25574,7 @@
         <v>119</v>
       </c>
       <c r="G1010" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H1010" s="6">
         <v>43909</v>
@@ -25598,7 +25603,7 @@
         <v>119</v>
       </c>
       <c r="G1011" s="5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H1011" s="6">
         <v>43909</v>
@@ -25654,7 +25659,7 @@
         <v>123</v>
       </c>
       <c r="G1013" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H1013" s="6">
         <v>43909</v>
@@ -25683,7 +25688,7 @@
         <v>119</v>
       </c>
       <c r="G1014" s="5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H1014" s="6">
         <v>43909</v>
@@ -25712,7 +25717,7 @@
         <v>119</v>
       </c>
       <c r="G1015" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H1015" s="6">
         <v>43909</v>
@@ -25741,7 +25746,7 @@
         <v>119</v>
       </c>
       <c r="G1016" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H1016" s="6">
         <v>43909</v>
@@ -25797,7 +25802,7 @@
         <v>120</v>
       </c>
       <c r="G1018" s="5" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="H1018" s="6">
         <v>43907</v>
@@ -25826,7 +25831,7 @@
         <v>120</v>
       </c>
       <c r="G1019" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="H1019" s="6">
         <v>43903</v>
@@ -25884,7 +25889,7 @@
         <v>127</v>
       </c>
       <c r="G1021" s="5" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H1021" s="6">
         <v>43907</v>
@@ -25934,7 +25939,7 @@
         <v>120</v>
       </c>
       <c r="G1023" s="5" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H1023" s="6">
         <v>43908</v>
@@ -26009,7 +26014,7 @@
         <v>125</v>
       </c>
       <c r="G1026" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H1026" s="6">
         <v>43911</v>
@@ -26080,7 +26085,7 @@
         <v>125</v>
       </c>
       <c r="G1029" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="H1029" s="6">
         <v>43909</v>
@@ -26415,7 +26420,7 @@
         <v>155</v>
       </c>
       <c r="G1042" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H1042" s="6">
         <v>43903</v>
@@ -26473,7 +26478,7 @@
         <v>131</v>
       </c>
       <c r="G1044" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H1044" s="6">
         <v>43907</v>
@@ -26502,7 +26507,7 @@
         <v>119</v>
       </c>
       <c r="G1045" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H1045" s="6">
         <v>43911</v>
@@ -26552,7 +26557,7 @@
         <v>122</v>
       </c>
       <c r="G1047" s="5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="H1047" s="6">
         <v>43909</v>
@@ -26602,7 +26607,7 @@
         <v>119</v>
       </c>
       <c r="G1049" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="H1049" s="6">
         <v>43906</v>
@@ -26685,7 +26690,7 @@
         <v>147</v>
       </c>
       <c r="G1052" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H1052" s="6">
         <v>43909</v>
@@ -26814,7 +26819,7 @@
         <v>119</v>
       </c>
       <c r="G1057" s="5" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H1057" s="6">
         <v>43906</v>
@@ -26870,7 +26875,7 @@
       </c>
       <c r="F1059" s="5"/>
       <c r="G1059" s="5" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H1059" s="6">
         <v>43898</v>
@@ -26918,7 +26923,7 @@
         <v>120</v>
       </c>
       <c r="G1061" s="5" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H1061" s="6"/>
       <c r="I1061" s="6">
@@ -26945,7 +26950,7 @@
         <v>146</v>
       </c>
       <c r="G1062" s="5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="H1062" s="6">
         <v>43910</v>
@@ -26974,7 +26979,7 @@
         <v>120</v>
       </c>
       <c r="G1063" s="5" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H1063" s="6">
         <v>43908</v>
@@ -27003,7 +27008,7 @@
         <v>120</v>
       </c>
       <c r="G1064" s="5" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H1064" s="6"/>
       <c r="I1064" s="6">
@@ -27030,7 +27035,7 @@
         <v>120</v>
       </c>
       <c r="G1065" s="5" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="H1065" s="6">
         <v>43905</v>
@@ -27207,7 +27212,7 @@
         <v>119</v>
       </c>
       <c r="G1072" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H1072" s="6">
         <v>43904</v>
@@ -27236,7 +27241,7 @@
         <v>120</v>
       </c>
       <c r="G1073" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H1073" s="6">
         <v>43908</v>
@@ -27265,7 +27270,7 @@
         <v>119</v>
       </c>
       <c r="G1074" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H1074" s="6">
         <v>43907</v>
@@ -27292,7 +27297,7 @@
       </c>
       <c r="F1075" s="5"/>
       <c r="G1075" s="5" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H1075" s="6">
         <v>43907</v>
@@ -27317,7 +27322,7 @@
       </c>
       <c r="F1076" s="5"/>
       <c r="G1076" s="5" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="H1076" s="6">
         <v>43905</v>
@@ -27469,7 +27474,7 @@
         <v>146</v>
       </c>
       <c r="G1082" s="5" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H1082" s="6">
         <v>43908</v>
@@ -27584,7 +27589,7 @@
       </c>
       <c r="F1087" s="5"/>
       <c r="G1087" s="5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H1087" s="6">
         <v>43905</v>
@@ -27609,7 +27614,7 @@
       </c>
       <c r="F1088" s="5"/>
       <c r="G1088" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H1088" s="6">
         <v>43908</v>
@@ -27636,7 +27641,7 @@
         <v>120</v>
       </c>
       <c r="G1089" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H1089" s="6">
         <v>43909</v>
@@ -27842,7 +27847,7 @@
         <v>123</v>
       </c>
       <c r="G1097" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="H1097" s="6">
         <v>43907</v>
@@ -27871,7 +27876,7 @@
         <v>131</v>
       </c>
       <c r="G1098" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H1098" s="6">
         <v>43902</v>
@@ -27919,7 +27924,7 @@
       </c>
       <c r="F1100" s="5"/>
       <c r="G1100" s="5" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="H1100" s="6">
         <v>43905</v>
@@ -27975,7 +27980,7 @@
         <v>123</v>
       </c>
       <c r="G1102" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H1102" s="6">
         <v>43907</v>
@@ -28033,7 +28038,7 @@
         <v>119</v>
       </c>
       <c r="G1104" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H1104" s="6">
         <v>43906</v>
@@ -28083,7 +28088,7 @@
         <v>146</v>
       </c>
       <c r="G1106" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H1106" s="6">
         <v>43908</v>
@@ -28141,7 +28146,7 @@
         <v>131</v>
       </c>
       <c r="G1108" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H1108" s="6">
         <v>43904</v>
@@ -28170,7 +28175,7 @@
         <v>119</v>
       </c>
       <c r="G1109" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H1109" s="6">
         <v>43903</v>
@@ -28197,7 +28202,7 @@
       </c>
       <c r="F1110" s="5"/>
       <c r="G1110" s="5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H1110" s="6">
         <v>43906</v>
@@ -28249,7 +28254,7 @@
         <v>119</v>
       </c>
       <c r="G1112" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H1112" s="6">
         <v>43903</v>
@@ -28278,7 +28283,7 @@
         <v>123</v>
       </c>
       <c r="G1113" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H1113" s="6"/>
       <c r="I1113" s="6">
@@ -28305,7 +28310,7 @@
         <v>123</v>
       </c>
       <c r="G1114" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H1114" s="6">
         <v>43905</v>
@@ -28384,7 +28389,7 @@
         <v>120</v>
       </c>
       <c r="G1117" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="H1117" s="6">
         <v>43904</v>
@@ -28413,7 +28418,7 @@
         <v>119</v>
       </c>
       <c r="G1118" s="5" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="H1118" s="6"/>
       <c r="I1118" s="6">
@@ -28440,7 +28445,7 @@
         <v>122</v>
       </c>
       <c r="G1119" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H1119" s="6">
         <v>43906</v>
@@ -28488,7 +28493,7 @@
       </c>
       <c r="F1121" s="5"/>
       <c r="G1121" s="5" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="H1121" s="6">
         <v>43903</v>
@@ -28646,7 +28651,7 @@
       </c>
       <c r="F1127" s="5"/>
       <c r="G1127" s="5" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H1127" s="6">
         <v>43894</v>
@@ -28673,7 +28678,7 @@
         <v>119</v>
       </c>
       <c r="G1128" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H1128" s="6"/>
       <c r="I1128" s="6">
@@ -28700,7 +28705,7 @@
         <v>127</v>
       </c>
       <c r="G1129" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H1129" s="6">
         <v>43904</v>
@@ -28779,7 +28784,7 @@
         <v>120</v>
       </c>
       <c r="G1132" s="5" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H1132" s="6">
         <v>43905</v>
@@ -28862,7 +28867,7 @@
         <v>123</v>
       </c>
       <c r="G1135" s="5" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H1135" s="6">
         <v>43903</v>
@@ -28891,7 +28896,7 @@
         <v>119</v>
       </c>
       <c r="G1136" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H1136" s="6">
         <v>43901</v>
@@ -28920,7 +28925,7 @@
         <v>131</v>
       </c>
       <c r="G1137" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H1137" s="6">
         <v>43903</v>
@@ -28949,7 +28954,7 @@
         <v>125</v>
       </c>
       <c r="G1138" s="5" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="H1138" s="6">
         <v>43906</v>
@@ -29053,7 +29058,7 @@
         <v>119</v>
       </c>
       <c r="G1142" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H1142" s="6">
         <v>43901</v>
@@ -29082,7 +29087,7 @@
         <v>119</v>
       </c>
       <c r="G1143" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H1143" s="6">
         <v>43900</v>
@@ -29111,7 +29116,7 @@
         <v>119</v>
       </c>
       <c r="G1144" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H1144" s="6">
         <v>43904</v>
@@ -29140,7 +29145,7 @@
         <v>119</v>
       </c>
       <c r="G1145" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H1145" s="6">
         <v>43904</v>
@@ -29198,7 +29203,7 @@
         <v>132</v>
       </c>
       <c r="G1147" s="5" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="H1147" s="6">
         <v>43905</v>
@@ -29227,7 +29232,7 @@
         <v>120</v>
       </c>
       <c r="G1148" s="5" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="H1148" s="6">
         <v>43898</v>
@@ -29306,7 +29311,7 @@
         <v>120</v>
       </c>
       <c r="G1151" s="5" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H1151" s="6">
         <v>43903</v>
@@ -29360,7 +29365,7 @@
         <v>119</v>
       </c>
       <c r="G1153" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H1153" s="6">
         <v>43895</v>
@@ -29431,7 +29436,7 @@
         <v>131</v>
       </c>
       <c r="G1156" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="H1156" s="6">
         <v>43886</v>
@@ -29460,7 +29465,7 @@
         <v>131</v>
       </c>
       <c r="G1157" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="H1157" s="6">
         <v>43886</v>
@@ -29537,7 +29542,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43977.375</v>
+        <v>43979.375</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -30360,7 +30365,7 @@
         <v>126</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H41" s="6">
         <v>43911</v>
@@ -31082,7 +31087,7 @@
         <v>120</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H75" s="6">
         <v>43911</v>
@@ -31616,7 +31621,7 @@
         <v>131</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H99" s="6">
         <v>43909</v>
@@ -31645,7 +31650,7 @@
         <v>125</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H100" s="6">
         <v>43913</v>
@@ -32620,7 +32625,7 @@
       </c>
       <c r="F145" s="5"/>
       <c r="G145" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H145" s="6">
         <v>43906</v>
@@ -34200,7 +34205,7 @@
         <v>120</v>
       </c>
       <c r="G219" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H219" s="6">
         <v>43908</v>
@@ -34651,7 +34656,7 @@
       </c>
       <c r="F240" s="5"/>
       <c r="G240" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H240" s="6">
         <v>43915</v>
@@ -35049,7 +35054,7 @@
       </c>
       <c r="F258" s="5"/>
       <c r="G258" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H258" s="6">
         <v>43912</v>
@@ -35244,7 +35249,7 @@
         <v>119</v>
       </c>
       <c r="G267" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H267" s="6"/>
       <c r="I267" s="6">
@@ -35338,7 +35343,7 @@
         <v>120</v>
       </c>
       <c r="G271" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H271" s="6">
         <v>43911</v>
@@ -35407,7 +35412,7 @@
       </c>
       <c r="F274" s="5"/>
       <c r="G274" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H274" s="6">
         <v>43913</v>
@@ -35670,7 +35675,7 @@
         <v>119</v>
       </c>
       <c r="G285" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H285" s="6">
         <v>43913</v>
@@ -35718,7 +35723,7 @@
       </c>
       <c r="F287" s="5"/>
       <c r="G287" s="5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H287" s="6">
         <v>43907</v>
@@ -35871,7 +35876,7 @@
         <v>120</v>
       </c>
       <c r="G294" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H294" s="6">
         <v>43908</v>
@@ -36047,7 +36052,7 @@
         <v>120</v>
       </c>
       <c r="G302" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H302" s="6">
         <v>43908</v>
@@ -36076,7 +36081,7 @@
         <v>139</v>
       </c>
       <c r="G303" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H303" s="6">
         <v>43909</v>
@@ -36247,7 +36252,7 @@
         <v>120</v>
       </c>
       <c r="G310" s="5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H310" s="6">
         <v>43909</v>
@@ -36452,7 +36457,7 @@
         <v>123</v>
       </c>
       <c r="G319" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H319" s="6">
         <v>43908</v>
@@ -36481,7 +36486,7 @@
         <v>123</v>
       </c>
       <c r="G320" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H320" s="6">
         <v>43908</v>
@@ -36510,7 +36515,7 @@
         <v>126</v>
       </c>
       <c r="G321" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H321" s="6">
         <v>43915</v>
@@ -36560,7 +36565,7 @@
         <v>147</v>
       </c>
       <c r="G323" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H323" s="6">
         <v>43909</v>
@@ -36673,7 +36678,7 @@
         <v>119</v>
       </c>
       <c r="G328" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H328" s="6">
         <v>43909</v>
@@ -36800,7 +36805,7 @@
         <v>119</v>
       </c>
       <c r="G333" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H333" s="6">
         <v>43907</v>
@@ -37281,7 +37286,7 @@
         <v>119</v>
       </c>
       <c r="G354" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H354" s="6">
         <v>43884</v>

</xml_diff>

<commit_message>
updated for the 29th May
</commit_message>
<xml_diff>
--- a/data/NZ_COVID19_data.xlsx
+++ b/data/NZ_COVID19_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\moh.govt.nz\dfs-userdata\userstate\iholmste\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21D0398B-7686-413F-AF1A-5E925A9F2826}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{03163058-D21F-46EF-B8A3-540A4CF7DD7D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8588" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8591" uniqueCount="333">
   <si>
     <t>BEKA76</t>
   </si>
@@ -554,6 +554,9 @@
   </si>
   <si>
     <t>NZ23</t>
+  </si>
+  <si>
+    <t>NZ610</t>
   </si>
   <si>
     <t>NZ102</t>
@@ -1403,7 +1406,7 @@
   </sheetPr>
   <dimension ref="A1:I1158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A452" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A444" workbookViewId="0">
       <selection activeCell="I476" sqref="I476"/>
     </sheetView>
   </sheetViews>
@@ -1428,7 +1431,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43979.375</v>
+        <v>43980.375</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -1896,7 +1899,7 @@
         <v>121</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="6">
@@ -5270,8 +5273,12 @@
         <v>115</v>
       </c>
       <c r="F171" s="5"/>
-      <c r="G171" s="5"/>
-      <c r="H171" s="6"/>
+      <c r="G171" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="H171" s="6">
+        <v>43911</v>
+      </c>
       <c r="I171" s="6"/>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
@@ -5550,7 +5557,7 @@
         <v>120</v>
       </c>
       <c r="G184" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H184" s="6">
         <v>43918</v>
@@ -5776,7 +5783,7 @@
         <v>126</v>
       </c>
       <c r="G194" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H194" s="6"/>
       <c r="I194" s="6">
@@ -5801,7 +5808,7 @@
       </c>
       <c r="F195" s="5"/>
       <c r="G195" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H195" s="6">
         <v>43916</v>
@@ -5891,7 +5898,7 @@
         <v>123</v>
       </c>
       <c r="G199" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H199" s="6">
         <v>43918</v>
@@ -5939,7 +5946,7 @@
       </c>
       <c r="F201" s="5"/>
       <c r="G201" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H201" s="6">
         <v>43913</v>
@@ -6045,7 +6052,7 @@
         <v>119</v>
       </c>
       <c r="G205" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H205" s="6">
         <v>43920</v>
@@ -6095,7 +6102,7 @@
         <v>122</v>
       </c>
       <c r="G207" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H207" s="6">
         <v>43912</v>
@@ -6485,7 +6492,7 @@
         <v>131</v>
       </c>
       <c r="G225" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H225" s="6">
         <v>43909</v>
@@ -6562,7 +6569,7 @@
       </c>
       <c r="F228" s="5"/>
       <c r="G228" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H228" s="6">
         <v>43921</v>
@@ -6750,7 +6757,7 @@
       </c>
       <c r="F236" s="5"/>
       <c r="G236" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H236" s="6">
         <v>43913</v>
@@ -6800,7 +6807,7 @@
       </c>
       <c r="F238" s="5"/>
       <c r="G238" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H238" s="6">
         <v>43913</v>
@@ -6848,7 +6855,7 @@
         <v>127</v>
       </c>
       <c r="G240" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H240" s="6">
         <v>43912</v>
@@ -7171,7 +7178,7 @@
         <v>120</v>
       </c>
       <c r="G255" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H255" s="6">
         <v>43913</v>
@@ -7783,7 +7790,7 @@
         <v>132</v>
       </c>
       <c r="G283" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H283" s="6">
         <v>43911</v>
@@ -7858,7 +7865,7 @@
         <v>133</v>
       </c>
       <c r="G286" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H286" s="6">
         <v>43911</v>
@@ -7956,7 +7963,7 @@
       </c>
       <c r="F290" s="5"/>
       <c r="G290" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H290" s="6">
         <v>43911</v>
@@ -7983,7 +7990,7 @@
         <v>120</v>
       </c>
       <c r="G291" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H291" s="6">
         <v>43909</v>
@@ -8186,7 +8193,7 @@
       </c>
       <c r="F300" s="5"/>
       <c r="G300" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H300" s="6">
         <v>43915</v>
@@ -8255,7 +8262,7 @@
         <v>120</v>
       </c>
       <c r="G303" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H303" s="6"/>
       <c r="I303" s="6">
@@ -8466,7 +8473,7 @@
         <v>120</v>
       </c>
       <c r="G312" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H312" s="6">
         <v>43910</v>
@@ -8579,7 +8586,7 @@
         <v>123</v>
       </c>
       <c r="G317" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H317" s="6">
         <v>43918</v>
@@ -8826,7 +8833,7 @@
         <v>135</v>
       </c>
       <c r="G328" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H328" s="6">
         <v>43914</v>
@@ -8854,8 +8861,12 @@
       <c r="F329" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="G329" s="5"/>
-      <c r="H329" s="6"/>
+      <c r="G329" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="H329" s="6">
+        <v>43917</v>
+      </c>
       <c r="I329" s="6">
         <v>43917</v>
       </c>
@@ -8879,8 +8890,12 @@
       <c r="F330" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="G330" s="5"/>
-      <c r="H330" s="6"/>
+      <c r="G330" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="H330" s="6">
+        <v>43917</v>
+      </c>
       <c r="I330" s="6">
         <v>43917</v>
       </c>
@@ -8903,7 +8918,7 @@
       </c>
       <c r="F331" s="5"/>
       <c r="G331" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H331" s="6">
         <v>43909</v>
@@ -8930,7 +8945,7 @@
         <v>131</v>
       </c>
       <c r="G332" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H332" s="6">
         <v>43909</v>
@@ -9068,7 +9083,7 @@
         <v>123</v>
       </c>
       <c r="G338" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H338" s="6"/>
       <c r="I338" s="6">
@@ -9095,7 +9110,7 @@
         <v>123</v>
       </c>
       <c r="G339" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H339" s="6">
         <v>43912</v>
@@ -9271,7 +9286,7 @@
         <v>123</v>
       </c>
       <c r="G347" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H347" s="6">
         <v>43913</v>
@@ -9665,7 +9680,7 @@
         <v>119</v>
       </c>
       <c r="G365" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H365" s="6">
         <v>43918</v>
@@ -9865,7 +9880,7 @@
         <v>123</v>
       </c>
       <c r="G373" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H373" s="6">
         <v>43905</v>
@@ -9978,7 +9993,7 @@
         <v>127</v>
       </c>
       <c r="G378" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H378" s="6">
         <v>43911</v>
@@ -10145,7 +10160,7 @@
         <v>119</v>
       </c>
       <c r="G385" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H385" s="6">
         <v>43914</v>
@@ -10174,7 +10189,7 @@
         <v>119</v>
       </c>
       <c r="G386" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H386" s="6">
         <v>43914</v>
@@ -10203,7 +10218,7 @@
         <v>120</v>
       </c>
       <c r="G387" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H387" s="6">
         <v>43914</v>
@@ -10232,7 +10247,7 @@
         <v>120</v>
       </c>
       <c r="G388" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H388" s="6">
         <v>43914</v>
@@ -10261,7 +10276,7 @@
         <v>132</v>
       </c>
       <c r="G389" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H389" s="6"/>
       <c r="I389" s="6">
@@ -10309,7 +10324,7 @@
         <v>120</v>
       </c>
       <c r="G391" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H391" s="6">
         <v>43908</v>
@@ -10497,7 +10512,7 @@
         <v>123</v>
       </c>
       <c r="G399" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H399" s="6">
         <v>43910</v>
@@ -11020,7 +11035,7 @@
         <v>119</v>
       </c>
       <c r="G422" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H422" s="6">
         <v>43908</v>
@@ -11091,7 +11106,7 @@
         <v>123</v>
       </c>
       <c r="G425" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H425" s="6">
         <v>43913</v>
@@ -11145,7 +11160,7 @@
         <v>119</v>
       </c>
       <c r="G427" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H427" s="6">
         <v>43913</v>
@@ -11288,7 +11303,7 @@
       </c>
       <c r="F432" s="5"/>
       <c r="G432" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H432" s="6">
         <v>43914</v>
@@ -11344,7 +11359,7 @@
         <v>137</v>
       </c>
       <c r="G434" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H434" s="6"/>
       <c r="I434" s="6">
@@ -11507,7 +11522,7 @@
       </c>
       <c r="F441" s="5"/>
       <c r="G441" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H441" s="6">
         <v>43912</v>
@@ -11563,7 +11578,7 @@
         <v>126</v>
       </c>
       <c r="G443" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H443" s="6">
         <v>43915</v>
@@ -11784,7 +11799,7 @@
         <v>120</v>
       </c>
       <c r="G452" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H452" s="6">
         <v>43913</v>
@@ -11897,7 +11912,7 @@
         <v>120</v>
       </c>
       <c r="G457" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H457" s="6">
         <v>43913</v>
@@ -12052,7 +12067,7 @@
         <v>120</v>
       </c>
       <c r="G464" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H464" s="6">
         <v>43913</v>
@@ -12081,7 +12096,7 @@
         <v>131</v>
       </c>
       <c r="G465" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H465" s="6">
         <v>43913</v>
@@ -12171,7 +12186,7 @@
       </c>
       <c r="F469" s="5"/>
       <c r="G469" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H469" s="6">
         <v>43908</v>
@@ -12342,7 +12357,7 @@
         <v>120</v>
       </c>
       <c r="G476" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H476" s="6">
         <v>43907</v>
@@ -12461,7 +12476,7 @@
         <v>119</v>
       </c>
       <c r="G481" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H481" s="6">
         <v>43907</v>
@@ -12511,7 +12526,7 @@
         <v>120</v>
       </c>
       <c r="G483" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H483" s="6">
         <v>43912</v>
@@ -12755,7 +12770,7 @@
       </c>
       <c r="F493" s="5"/>
       <c r="G493" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H493" s="6">
         <v>43918</v>
@@ -12801,7 +12816,7 @@
       </c>
       <c r="F495" s="5"/>
       <c r="G495" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H495" s="6">
         <v>43913</v>
@@ -12828,7 +12843,7 @@
         <v>119</v>
       </c>
       <c r="G496" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H496" s="6">
         <v>43913</v>
@@ -12876,7 +12891,7 @@
       </c>
       <c r="F498" s="5"/>
       <c r="G498" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H498" s="6">
         <v>43909</v>
@@ -12903,7 +12918,7 @@
         <v>131</v>
       </c>
       <c r="G499" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H499" s="6">
         <v>43909</v>
@@ -12980,7 +12995,7 @@
       </c>
       <c r="F502" s="5"/>
       <c r="G502" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H502" s="6">
         <v>43915</v>
@@ -13007,7 +13022,7 @@
         <v>122</v>
       </c>
       <c r="G503" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H503" s="6"/>
       <c r="I503" s="6">
@@ -13055,7 +13070,7 @@
         <v>122</v>
       </c>
       <c r="G505" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H505" s="6"/>
       <c r="I505" s="6">
@@ -13103,7 +13118,7 @@
         <v>120</v>
       </c>
       <c r="G507" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H507" s="6">
         <v>43913</v>
@@ -13132,7 +13147,7 @@
         <v>120</v>
       </c>
       <c r="G508" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H508" s="6">
         <v>43913</v>
@@ -13243,7 +13258,7 @@
       </c>
       <c r="F513" s="5"/>
       <c r="G513" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H513" s="6">
         <v>43912</v>
@@ -13293,7 +13308,7 @@
         <v>120</v>
       </c>
       <c r="G515" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H515" s="6">
         <v>43910</v>
@@ -14184,7 +14199,7 @@
       </c>
       <c r="F554" s="5"/>
       <c r="G554" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H554" s="6">
         <v>43910</v>
@@ -14211,7 +14226,7 @@
         <v>123</v>
       </c>
       <c r="G555" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H555" s="6">
         <v>43913</v>
@@ -14265,7 +14280,7 @@
         <v>119</v>
       </c>
       <c r="G557" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H557" s="6"/>
       <c r="I557" s="6">
@@ -14397,7 +14412,7 @@
         <v>119</v>
       </c>
       <c r="G563" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H563" s="6">
         <v>43912</v>
@@ -14470,7 +14485,7 @@
       </c>
       <c r="F566" s="5"/>
       <c r="G566" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H566" s="6">
         <v>43905</v>
@@ -14560,7 +14575,7 @@
         <v>128</v>
       </c>
       <c r="G570" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H570" s="6"/>
       <c r="I570" s="6">
@@ -14587,7 +14602,7 @@
         <v>120</v>
       </c>
       <c r="G571" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H571" s="6">
         <v>43909</v>
@@ -15012,7 +15027,7 @@
         <v>139</v>
       </c>
       <c r="G590" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H590" s="6">
         <v>43907</v>
@@ -15233,7 +15248,7 @@
         <v>120</v>
       </c>
       <c r="G599" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H599" s="6">
         <v>43908</v>
@@ -15262,7 +15277,7 @@
         <v>119</v>
       </c>
       <c r="G600" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H600" s="6">
         <v>43913</v>
@@ -15316,7 +15331,7 @@
         <v>131</v>
       </c>
       <c r="G602" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H602" s="6">
         <v>43909</v>
@@ -15366,7 +15381,7 @@
         <v>120</v>
       </c>
       <c r="G604" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H604" s="6">
         <v>43914</v>
@@ -15395,7 +15410,7 @@
         <v>127</v>
       </c>
       <c r="G605" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H605" s="6">
         <v>43910</v>
@@ -15468,7 +15483,7 @@
         <v>127</v>
       </c>
       <c r="G608" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H608" s="6">
         <v>43912</v>
@@ -15516,7 +15531,7 @@
       </c>
       <c r="F610" s="5"/>
       <c r="G610" s="5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H610" s="6">
         <v>43915</v>
@@ -15643,7 +15658,7 @@
         <v>120</v>
       </c>
       <c r="G615" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H615" s="6">
         <v>43909</v>
@@ -15672,7 +15687,7 @@
         <v>132</v>
       </c>
       <c r="G616" s="5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H616" s="6"/>
       <c r="I616" s="6">
@@ -15699,7 +15714,7 @@
         <v>126</v>
       </c>
       <c r="G617" s="5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="H617" s="6">
         <v>43913</v>
@@ -16181,7 +16196,7 @@
       </c>
       <c r="F639" s="5"/>
       <c r="G639" s="5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H639" s="6">
         <v>43913</v>
@@ -16447,7 +16462,7 @@
         <v>139</v>
       </c>
       <c r="G651" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H651" s="6">
         <v>43909</v>
@@ -16697,7 +16712,7 @@
         <v>119</v>
       </c>
       <c r="G661" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H661" s="6">
         <v>43908</v>
@@ -16901,7 +16916,7 @@
         <v>119</v>
       </c>
       <c r="G669" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H669" s="6">
         <v>43905</v>
@@ -17043,7 +17058,7 @@
         <v>120</v>
       </c>
       <c r="G675" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H675" s="6">
         <v>43913</v>
@@ -17072,7 +17087,7 @@
         <v>140</v>
       </c>
       <c r="G676" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H676" s="6">
         <v>43906</v>
@@ -17101,7 +17116,7 @@
         <v>118</v>
       </c>
       <c r="G677" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H677" s="6">
         <v>43905</v>
@@ -17130,7 +17145,7 @@
         <v>123</v>
       </c>
       <c r="G678" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H678" s="6">
         <v>43913</v>
@@ -17159,7 +17174,7 @@
         <v>120</v>
       </c>
       <c r="G679" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H679" s="6">
         <v>43914</v>
@@ -17213,7 +17228,7 @@
         <v>120</v>
       </c>
       <c r="G681" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H681" s="6">
         <v>43914</v>
@@ -17242,7 +17257,7 @@
         <v>127</v>
       </c>
       <c r="G682" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H682" s="6">
         <v>43914</v>
@@ -17271,7 +17286,7 @@
         <v>120</v>
       </c>
       <c r="G683" s="5" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H683" s="6">
         <v>43915</v>
@@ -17300,7 +17315,7 @@
         <v>127</v>
       </c>
       <c r="G684" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H684" s="6">
         <v>43912</v>
@@ -17350,7 +17365,7 @@
         <v>127</v>
       </c>
       <c r="G686" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H686" s="6">
         <v>43907</v>
@@ -17542,7 +17557,7 @@
         <v>125</v>
       </c>
       <c r="G694" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H694" s="6"/>
       <c r="I694" s="6">
@@ -17567,7 +17582,7 @@
       </c>
       <c r="F695" s="5"/>
       <c r="G695" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H695" s="6">
         <v>43908</v>
@@ -17621,7 +17636,7 @@
         <v>119</v>
       </c>
       <c r="G697" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H697" s="6">
         <v>43907</v>
@@ -17717,7 +17732,7 @@
         <v>123</v>
       </c>
       <c r="G701" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H701" s="6">
         <v>43909</v>
@@ -17849,7 +17864,7 @@
       </c>
       <c r="F707" s="5"/>
       <c r="G707" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H707" s="6">
         <v>43906</v>
@@ -17878,7 +17893,7 @@
         <v>123</v>
       </c>
       <c r="G708" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H708" s="6">
         <v>43910</v>
@@ -17928,7 +17943,7 @@
         <v>118</v>
       </c>
       <c r="G710" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H710" s="6">
         <v>43909</v>
@@ -18162,7 +18177,7 @@
         <v>119</v>
       </c>
       <c r="G720" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H720" s="6">
         <v>43908</v>
@@ -18279,7 +18294,7 @@
         <v>119</v>
       </c>
       <c r="G725" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H725" s="6">
         <v>43908</v>
@@ -18379,7 +18394,7 @@
         <v>139</v>
       </c>
       <c r="G729" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H729" s="6">
         <v>43909</v>
@@ -18458,7 +18473,7 @@
         <v>119</v>
       </c>
       <c r="G732" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H732" s="6">
         <v>43908</v>
@@ -18487,7 +18502,7 @@
         <v>127</v>
       </c>
       <c r="G733" s="5" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H733" s="6">
         <v>43913</v>
@@ -18514,7 +18529,7 @@
       </c>
       <c r="F734" s="5"/>
       <c r="G734" s="5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H734" s="6">
         <v>43908</v>
@@ -18539,7 +18554,7 @@
       </c>
       <c r="F735" s="5"/>
       <c r="G735" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H735" s="6">
         <v>43907</v>
@@ -18595,7 +18610,7 @@
         <v>123</v>
       </c>
       <c r="G737" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H737" s="6">
         <v>43910</v>
@@ -18622,7 +18637,7 @@
       </c>
       <c r="F738" s="5"/>
       <c r="G738" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="H738" s="6">
         <v>43913</v>
@@ -18649,7 +18664,7 @@
         <v>123</v>
       </c>
       <c r="G739" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H739" s="6">
         <v>43912</v>
@@ -18676,7 +18691,7 @@
       </c>
       <c r="F740" s="5"/>
       <c r="G740" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="H740" s="6">
         <v>43913</v>
@@ -18753,7 +18768,7 @@
         <v>119</v>
       </c>
       <c r="G743" s="5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H743" s="6">
         <v>43912</v>
@@ -18780,7 +18795,7 @@
       </c>
       <c r="F744" s="5"/>
       <c r="G744" s="5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="H744" s="6">
         <v>43910</v>
@@ -18828,7 +18843,7 @@
         <v>125</v>
       </c>
       <c r="G746" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H746" s="6">
         <v>43912</v>
@@ -18857,7 +18872,7 @@
         <v>128</v>
       </c>
       <c r="G747" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H747" s="6">
         <v>43912</v>
@@ -18886,7 +18901,7 @@
         <v>131</v>
       </c>
       <c r="G748" s="5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H748" s="6">
         <v>43910</v>
@@ -18915,7 +18930,7 @@
         <v>131</v>
       </c>
       <c r="G749" s="5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H749" s="6">
         <v>43910</v>
@@ -18944,7 +18959,7 @@
         <v>119</v>
       </c>
       <c r="G750" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H750" s="6">
         <v>43902</v>
@@ -19013,7 +19028,7 @@
       </c>
       <c r="F753" s="5"/>
       <c r="G753" s="5" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H753" s="6">
         <v>43909</v>
@@ -19063,7 +19078,7 @@
         <v>119</v>
       </c>
       <c r="G755" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H755" s="6">
         <v>43907</v>
@@ -19134,7 +19149,7 @@
         <v>123</v>
       </c>
       <c r="G758" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H758" s="6">
         <v>43910</v>
@@ -19373,7 +19388,7 @@
         <v>119</v>
       </c>
       <c r="G769" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H769" s="6"/>
       <c r="I769" s="6">
@@ -19586,7 +19601,7 @@
         <v>123</v>
       </c>
       <c r="G778" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H778" s="6">
         <v>43908</v>
@@ -19615,7 +19630,7 @@
         <v>131</v>
       </c>
       <c r="G779" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H779" s="6">
         <v>43914</v>
@@ -19791,7 +19806,7 @@
         <v>123</v>
       </c>
       <c r="G787" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H787" s="6"/>
       <c r="I787" s="6">
@@ -19887,7 +19902,7 @@
         <v>129</v>
       </c>
       <c r="G791" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H791" s="6">
         <v>43915</v>
@@ -19941,7 +19956,7 @@
         <v>119</v>
       </c>
       <c r="G793" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H793" s="6">
         <v>43912</v>
@@ -19970,7 +19985,7 @@
         <v>119</v>
       </c>
       <c r="G794" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H794" s="6">
         <v>43912</v>
@@ -19999,7 +20014,7 @@
         <v>119</v>
       </c>
       <c r="G795" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H795" s="6">
         <v>43912</v>
@@ -20049,7 +20064,7 @@
         <v>120</v>
       </c>
       <c r="G797" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="H797" s="6">
         <v>43914</v>
@@ -20078,7 +20093,7 @@
         <v>120</v>
       </c>
       <c r="G798" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="H798" s="6">
         <v>43914</v>
@@ -20107,7 +20122,7 @@
         <v>119</v>
       </c>
       <c r="G799" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H799" s="6">
         <v>43912</v>
@@ -20245,7 +20260,7 @@
         <v>119</v>
       </c>
       <c r="G805" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H805" s="6">
         <v>43908</v>
@@ -20299,7 +20314,7 @@
         <v>125</v>
       </c>
       <c r="G807" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H807" s="6">
         <v>43913</v>
@@ -20424,7 +20439,7 @@
         <v>120</v>
       </c>
       <c r="G812" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H812" s="6">
         <v>43904</v>
@@ -20453,7 +20468,7 @@
         <v>120</v>
       </c>
       <c r="G813" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H813" s="6">
         <v>43909</v>
@@ -20482,7 +20497,7 @@
         <v>143</v>
       </c>
       <c r="G814" s="5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="H814" s="6">
         <v>43908</v>
@@ -20511,7 +20526,7 @@
         <v>126</v>
       </c>
       <c r="G815" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H815" s="6">
         <v>43908</v>
@@ -20540,7 +20555,7 @@
         <v>119</v>
       </c>
       <c r="G816" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="H816" s="6">
         <v>43909</v>
@@ -20640,7 +20655,7 @@
         <v>120</v>
       </c>
       <c r="G820" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H820" s="6">
         <v>43913</v>
@@ -20669,7 +20684,7 @@
         <v>119</v>
       </c>
       <c r="G821" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H821" s="6">
         <v>43909</v>
@@ -20698,7 +20713,7 @@
         <v>120</v>
       </c>
       <c r="G822" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H822" s="6">
         <v>43914</v>
@@ -20727,7 +20742,7 @@
         <v>119</v>
       </c>
       <c r="G823" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H823" s="6">
         <v>43910</v>
@@ -20806,7 +20821,7 @@
         <v>119</v>
       </c>
       <c r="G826" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H826" s="6">
         <v>43915</v>
@@ -20835,7 +20850,7 @@
         <v>120</v>
       </c>
       <c r="G827" s="5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H827" s="6">
         <v>43910</v>
@@ -20864,7 +20879,7 @@
         <v>120</v>
       </c>
       <c r="G828" s="5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H828" s="6">
         <v>43910</v>
@@ -20914,7 +20929,7 @@
         <v>127</v>
       </c>
       <c r="G830" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H830" s="6">
         <v>43911</v>
@@ -20993,7 +21008,7 @@
         <v>128</v>
       </c>
       <c r="G833" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H833" s="6">
         <v>43909</v>
@@ -21022,7 +21037,7 @@
         <v>125</v>
       </c>
       <c r="G834" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="H834" s="6">
         <v>43913</v>
@@ -21124,7 +21139,7 @@
         <v>119</v>
       </c>
       <c r="G838" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="H838" s="6">
         <v>43911</v>
@@ -21153,7 +21168,7 @@
         <v>119</v>
       </c>
       <c r="G839" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H839" s="6"/>
       <c r="I839" s="6">
@@ -21222,7 +21237,7 @@
         <v>146</v>
       </c>
       <c r="G842" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H842" s="6">
         <v>43906</v>
@@ -21251,7 +21266,7 @@
         <v>119</v>
       </c>
       <c r="G843" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H843" s="6">
         <v>43910</v>
@@ -21395,7 +21410,7 @@
       </c>
       <c r="F849" s="5"/>
       <c r="G849" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H849" s="6">
         <v>43910</v>
@@ -21424,7 +21439,7 @@
         <v>130</v>
       </c>
       <c r="G850" s="5" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H850" s="6">
         <v>43908</v>
@@ -21453,7 +21468,7 @@
         <v>120</v>
       </c>
       <c r="G851" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H851" s="6">
         <v>43908</v>
@@ -21561,7 +21576,7 @@
         <v>147</v>
       </c>
       <c r="G855" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H855" s="6">
         <v>43909</v>
@@ -21590,7 +21605,7 @@
         <v>119</v>
       </c>
       <c r="G856" s="5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H856" s="6">
         <v>43913</v>
@@ -21690,7 +21705,7 @@
         <v>120</v>
       </c>
       <c r="G860" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H860" s="6">
         <v>43908</v>
@@ -21744,7 +21759,7 @@
         <v>119</v>
       </c>
       <c r="G862" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H862" s="6">
         <v>43909</v>
@@ -21861,7 +21876,7 @@
         <v>131</v>
       </c>
       <c r="G867" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H867" s="6">
         <v>43907</v>
@@ -21990,7 +22005,7 @@
         <v>147</v>
       </c>
       <c r="G872" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="H872" s="6">
         <v>43905</v>
@@ -22019,7 +22034,7 @@
         <v>119</v>
       </c>
       <c r="G873" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H873" s="6">
         <v>43905</v>
@@ -22077,7 +22092,7 @@
         <v>139</v>
       </c>
       <c r="G875" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H875" s="6">
         <v>43909</v>
@@ -22106,7 +22121,7 @@
         <v>120</v>
       </c>
       <c r="G876" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H876" s="6"/>
       <c r="I876" s="6">
@@ -22133,7 +22148,7 @@
         <v>119</v>
       </c>
       <c r="G877" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H877" s="6">
         <v>43910</v>
@@ -22204,7 +22219,7 @@
         <v>120</v>
       </c>
       <c r="G880" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H880" s="6">
         <v>43914</v>
@@ -22254,7 +22269,7 @@
         <v>120</v>
       </c>
       <c r="G882" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="H882" s="6">
         <v>43911</v>
@@ -22283,7 +22298,7 @@
         <v>126</v>
       </c>
       <c r="G883" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H883" s="6">
         <v>43914</v>
@@ -22312,7 +22327,7 @@
         <v>127</v>
       </c>
       <c r="G884" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H884" s="6">
         <v>43911</v>
@@ -22341,7 +22356,7 @@
         <v>119</v>
       </c>
       <c r="G885" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H885" s="6">
         <v>43909</v>
@@ -22533,7 +22548,7 @@
         <v>148</v>
       </c>
       <c r="G893" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H893" s="6">
         <v>43906</v>
@@ -22562,7 +22577,7 @@
         <v>148</v>
       </c>
       <c r="G894" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H894" s="6">
         <v>43906</v>
@@ -22639,7 +22654,7 @@
         <v>127</v>
       </c>
       <c r="G897" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="H897" s="6">
         <v>43909</v>
@@ -22691,7 +22706,7 @@
       </c>
       <c r="F899" s="5"/>
       <c r="G899" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H899" s="6">
         <v>43908</v>
@@ -22872,7 +22887,7 @@
         <v>127</v>
       </c>
       <c r="G906" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="H906" s="6">
         <v>43909</v>
@@ -22943,7 +22958,7 @@
         <v>150</v>
       </c>
       <c r="G909" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H909" s="6"/>
       <c r="I909" s="6">
@@ -22970,7 +22985,7 @@
         <v>150</v>
       </c>
       <c r="G910" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="H910" s="6">
         <v>43909</v>
@@ -22997,7 +23012,7 @@
       </c>
       <c r="F911" s="5"/>
       <c r="G911" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H911" s="6">
         <v>43909</v>
@@ -23208,7 +23223,7 @@
         <v>131</v>
       </c>
       <c r="G920" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H920" s="6">
         <v>43905</v>
@@ -23279,7 +23294,7 @@
         <v>120</v>
       </c>
       <c r="G923" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="H923" s="6">
         <v>43912</v>
@@ -23396,7 +23411,7 @@
         <v>122</v>
       </c>
       <c r="G928" s="5" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H928" s="6">
         <v>43901</v>
@@ -23475,7 +23490,7 @@
         <v>119</v>
       </c>
       <c r="G931" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H931" s="6">
         <v>43907</v>
@@ -23527,7 +23542,7 @@
         <v>120</v>
       </c>
       <c r="G933" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="H933" s="6">
         <v>43912</v>
@@ -23585,7 +23600,7 @@
         <v>119</v>
       </c>
       <c r="G935" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H935" s="6">
         <v>43910</v>
@@ -23656,7 +23671,7 @@
         <v>145</v>
       </c>
       <c r="G938" s="5" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H938" s="6">
         <v>43905</v>
@@ -23735,7 +23750,7 @@
         <v>128</v>
       </c>
       <c r="G941" s="5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H941" s="6">
         <v>43903</v>
@@ -23764,7 +23779,7 @@
         <v>120</v>
       </c>
       <c r="G942" s="5" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="H942" s="6">
         <v>43909</v>
@@ -23793,7 +23808,7 @@
         <v>119</v>
       </c>
       <c r="G943" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H943" s="6">
         <v>43907</v>
@@ -23851,7 +23866,7 @@
         <v>119</v>
       </c>
       <c r="G945" s="5" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="H945" s="6">
         <v>43911</v>
@@ -23951,7 +23966,7 @@
         <v>119</v>
       </c>
       <c r="G949" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H949" s="6">
         <v>43905</v>
@@ -23980,7 +23995,7 @@
         <v>119</v>
       </c>
       <c r="G950" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H950" s="6">
         <v>43909</v>
@@ -24030,7 +24045,7 @@
         <v>118</v>
       </c>
       <c r="G952" s="5" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="H952" s="6">
         <v>43910</v>
@@ -24059,7 +24074,7 @@
         <v>141</v>
       </c>
       <c r="G953" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H953" s="6">
         <v>43910</v>
@@ -24088,7 +24103,7 @@
         <v>123</v>
       </c>
       <c r="G954" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H954" s="6">
         <v>43909</v>
@@ -24117,7 +24132,7 @@
         <v>123</v>
       </c>
       <c r="G955" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H955" s="6">
         <v>43910</v>
@@ -24146,7 +24161,7 @@
         <v>119</v>
       </c>
       <c r="G956" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H956" s="6">
         <v>43909</v>
@@ -24221,7 +24236,7 @@
         <v>119</v>
       </c>
       <c r="G959" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H959" s="6">
         <v>43907</v>
@@ -24250,7 +24265,7 @@
         <v>119</v>
       </c>
       <c r="G960" s="5" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="H960" s="6">
         <v>43910</v>
@@ -24300,7 +24315,7 @@
         <v>119</v>
       </c>
       <c r="G962" s="5" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H962" s="6">
         <v>43910</v>
@@ -24329,7 +24344,7 @@
         <v>120</v>
       </c>
       <c r="G963" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H963" s="6">
         <v>43911</v>
@@ -24358,7 +24373,7 @@
         <v>120</v>
       </c>
       <c r="G964" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="H964" s="6">
         <v>43910</v>
@@ -24387,7 +24402,7 @@
         <v>127</v>
       </c>
       <c r="G965" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H965" s="6">
         <v>43908</v>
@@ -24416,7 +24431,7 @@
         <v>119</v>
       </c>
       <c r="G966" s="5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H966" s="6">
         <v>43910</v>
@@ -24445,7 +24460,7 @@
         <v>119</v>
       </c>
       <c r="G967" s="5" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H967" s="6">
         <v>43910</v>
@@ -24638,7 +24653,7 @@
         <v>120</v>
       </c>
       <c r="G974" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H974" s="6"/>
       <c r="I974" s="6">
@@ -24686,7 +24701,7 @@
         <v>132</v>
       </c>
       <c r="G976" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="H976" s="6">
         <v>43906</v>
@@ -24765,7 +24780,7 @@
         <v>119</v>
       </c>
       <c r="G979" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H979" s="6">
         <v>43909</v>
@@ -24794,7 +24809,7 @@
         <v>146</v>
       </c>
       <c r="G980" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H980" s="6">
         <v>43913</v>
@@ -24823,7 +24838,7 @@
         <v>123</v>
       </c>
       <c r="G981" s="5" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H981" s="6">
         <v>43911</v>
@@ -24898,7 +24913,7 @@
         <v>154</v>
       </c>
       <c r="G984" s="5" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H984" s="6">
         <v>43909</v>
@@ -24948,7 +24963,7 @@
         <v>123</v>
       </c>
       <c r="G986" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H986" s="6">
         <v>43906</v>
@@ -25023,7 +25038,7 @@
         <v>120</v>
       </c>
       <c r="G989" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H989" s="6">
         <v>43910</v>
@@ -25073,7 +25088,7 @@
         <v>119</v>
       </c>
       <c r="G991" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H991" s="6">
         <v>43906</v>
@@ -25102,7 +25117,7 @@
         <v>119</v>
       </c>
       <c r="G992" s="5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="H992" s="6">
         <v>43907</v>
@@ -25252,7 +25267,7 @@
         <v>145</v>
       </c>
       <c r="G998" s="5" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H998" s="6">
         <v>43905</v>
@@ -25302,7 +25317,7 @@
         <v>120</v>
       </c>
       <c r="G1000" s="5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="H1000" s="6">
         <v>43909</v>
@@ -25360,7 +25375,7 @@
         <v>147</v>
       </c>
       <c r="G1002" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="H1002" s="6">
         <v>43905</v>
@@ -25389,7 +25404,7 @@
         <v>119</v>
       </c>
       <c r="G1003" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H1003" s="6">
         <v>43907</v>
@@ -25418,7 +25433,7 @@
         <v>131</v>
       </c>
       <c r="G1004" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H1004" s="6">
         <v>43911</v>
@@ -25447,7 +25462,7 @@
         <v>119</v>
       </c>
       <c r="G1005" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H1005" s="6">
         <v>43906</v>
@@ -25545,7 +25560,7 @@
         <v>131</v>
       </c>
       <c r="G1009" s="5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H1009" s="6">
         <v>43909</v>
@@ -25574,7 +25589,7 @@
         <v>119</v>
       </c>
       <c r="G1010" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H1010" s="6">
         <v>43909</v>
@@ -25603,7 +25618,7 @@
         <v>119</v>
       </c>
       <c r="G1011" s="5" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="H1011" s="6">
         <v>43909</v>
@@ -25659,7 +25674,7 @@
         <v>123</v>
       </c>
       <c r="G1013" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H1013" s="6">
         <v>43909</v>
@@ -25688,7 +25703,7 @@
         <v>119</v>
       </c>
       <c r="G1014" s="5" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="H1014" s="6">
         <v>43909</v>
@@ -25717,7 +25732,7 @@
         <v>119</v>
       </c>
       <c r="G1015" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H1015" s="6">
         <v>43909</v>
@@ -25746,7 +25761,7 @@
         <v>119</v>
       </c>
       <c r="G1016" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H1016" s="6">
         <v>43909</v>
@@ -25802,7 +25817,7 @@
         <v>120</v>
       </c>
       <c r="G1018" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="H1018" s="6">
         <v>43907</v>
@@ -25831,7 +25846,7 @@
         <v>120</v>
       </c>
       <c r="G1019" s="5" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H1019" s="6">
         <v>43903</v>
@@ -25889,7 +25904,7 @@
         <v>127</v>
       </c>
       <c r="G1021" s="5" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H1021" s="6">
         <v>43907</v>
@@ -25939,7 +25954,7 @@
         <v>120</v>
       </c>
       <c r="G1023" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="H1023" s="6">
         <v>43908</v>
@@ -26014,7 +26029,7 @@
         <v>125</v>
       </c>
       <c r="G1026" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H1026" s="6">
         <v>43911</v>
@@ -26085,7 +26100,7 @@
         <v>125</v>
       </c>
       <c r="G1029" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="H1029" s="6">
         <v>43909</v>
@@ -26420,7 +26435,7 @@
         <v>155</v>
       </c>
       <c r="G1042" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H1042" s="6">
         <v>43903</v>
@@ -26478,7 +26493,7 @@
         <v>131</v>
       </c>
       <c r="G1044" s="5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H1044" s="6">
         <v>43907</v>
@@ -26507,7 +26522,7 @@
         <v>119</v>
       </c>
       <c r="G1045" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H1045" s="6">
         <v>43911</v>
@@ -26557,7 +26572,7 @@
         <v>122</v>
       </c>
       <c r="G1047" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H1047" s="6">
         <v>43909</v>
@@ -26607,7 +26622,7 @@
         <v>119</v>
       </c>
       <c r="G1049" s="5" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H1049" s="6">
         <v>43906</v>
@@ -26690,7 +26705,7 @@
         <v>147</v>
       </c>
       <c r="G1052" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H1052" s="6">
         <v>43909</v>
@@ -26819,7 +26834,7 @@
         <v>119</v>
       </c>
       <c r="G1057" s="5" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H1057" s="6">
         <v>43906</v>
@@ -26875,7 +26890,7 @@
       </c>
       <c r="F1059" s="5"/>
       <c r="G1059" s="5" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H1059" s="6">
         <v>43898</v>
@@ -26923,7 +26938,7 @@
         <v>120</v>
       </c>
       <c r="G1061" s="5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="H1061" s="6"/>
       <c r="I1061" s="6">
@@ -26950,7 +26965,7 @@
         <v>146</v>
       </c>
       <c r="G1062" s="5" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="H1062" s="6">
         <v>43910</v>
@@ -26979,7 +26994,7 @@
         <v>120</v>
       </c>
       <c r="G1063" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="H1063" s="6">
         <v>43908</v>
@@ -27008,7 +27023,7 @@
         <v>120</v>
       </c>
       <c r="G1064" s="5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="H1064" s="6"/>
       <c r="I1064" s="6">
@@ -27035,7 +27050,7 @@
         <v>120</v>
       </c>
       <c r="G1065" s="5" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H1065" s="6">
         <v>43905</v>
@@ -27212,7 +27227,7 @@
         <v>119</v>
       </c>
       <c r="G1072" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H1072" s="6">
         <v>43904</v>
@@ -27241,7 +27256,7 @@
         <v>120</v>
       </c>
       <c r="G1073" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H1073" s="6">
         <v>43908</v>
@@ -27270,7 +27285,7 @@
         <v>119</v>
       </c>
       <c r="G1074" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H1074" s="6">
         <v>43907</v>
@@ -27297,7 +27312,7 @@
       </c>
       <c r="F1075" s="5"/>
       <c r="G1075" s="5" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="H1075" s="6">
         <v>43907</v>
@@ -27322,7 +27337,7 @@
       </c>
       <c r="F1076" s="5"/>
       <c r="G1076" s="5" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H1076" s="6">
         <v>43905</v>
@@ -27474,7 +27489,7 @@
         <v>146</v>
       </c>
       <c r="G1082" s="5" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="H1082" s="6">
         <v>43908</v>
@@ -27589,7 +27604,7 @@
       </c>
       <c r="F1087" s="5"/>
       <c r="G1087" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H1087" s="6">
         <v>43905</v>
@@ -27614,7 +27629,7 @@
       </c>
       <c r="F1088" s="5"/>
       <c r="G1088" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H1088" s="6">
         <v>43908</v>
@@ -27641,7 +27656,7 @@
         <v>120</v>
       </c>
       <c r="G1089" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H1089" s="6">
         <v>43909</v>
@@ -27847,7 +27862,7 @@
         <v>123</v>
       </c>
       <c r="G1097" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H1097" s="6">
         <v>43907</v>
@@ -27876,7 +27891,7 @@
         <v>131</v>
       </c>
       <c r="G1098" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H1098" s="6">
         <v>43902</v>
@@ -27924,7 +27939,7 @@
       </c>
       <c r="F1100" s="5"/>
       <c r="G1100" s="5" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="H1100" s="6">
         <v>43905</v>
@@ -27980,7 +27995,7 @@
         <v>123</v>
       </c>
       <c r="G1102" s="5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H1102" s="6">
         <v>43907</v>
@@ -28038,7 +28053,7 @@
         <v>119</v>
       </c>
       <c r="G1104" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="H1104" s="6">
         <v>43906</v>
@@ -28088,7 +28103,7 @@
         <v>146</v>
       </c>
       <c r="G1106" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H1106" s="6">
         <v>43908</v>
@@ -28146,7 +28161,7 @@
         <v>131</v>
       </c>
       <c r="G1108" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H1108" s="6">
         <v>43904</v>
@@ -28175,7 +28190,7 @@
         <v>119</v>
       </c>
       <c r="G1109" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H1109" s="6">
         <v>43903</v>
@@ -28202,7 +28217,7 @@
       </c>
       <c r="F1110" s="5"/>
       <c r="G1110" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H1110" s="6">
         <v>43906</v>
@@ -28254,7 +28269,7 @@
         <v>119</v>
       </c>
       <c r="G1112" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H1112" s="6">
         <v>43903</v>
@@ -28283,7 +28298,7 @@
         <v>123</v>
       </c>
       <c r="G1113" s="5" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H1113" s="6"/>
       <c r="I1113" s="6">
@@ -28310,7 +28325,7 @@
         <v>123</v>
       </c>
       <c r="G1114" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H1114" s="6">
         <v>43905</v>
@@ -28389,7 +28404,7 @@
         <v>120</v>
       </c>
       <c r="G1117" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="H1117" s="6">
         <v>43904</v>
@@ -28418,7 +28433,7 @@
         <v>119</v>
       </c>
       <c r="G1118" s="5" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="H1118" s="6"/>
       <c r="I1118" s="6">
@@ -28445,7 +28460,7 @@
         <v>122</v>
       </c>
       <c r="G1119" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H1119" s="6">
         <v>43906</v>
@@ -28493,7 +28508,7 @@
       </c>
       <c r="F1121" s="5"/>
       <c r="G1121" s="5" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H1121" s="6">
         <v>43903</v>
@@ -28651,7 +28666,7 @@
       </c>
       <c r="F1127" s="5"/>
       <c r="G1127" s="5" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H1127" s="6">
         <v>43894</v>
@@ -28678,7 +28693,7 @@
         <v>119</v>
       </c>
       <c r="G1128" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H1128" s="6"/>
       <c r="I1128" s="6">
@@ -28705,7 +28720,7 @@
         <v>127</v>
       </c>
       <c r="G1129" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H1129" s="6">
         <v>43904</v>
@@ -28784,7 +28799,7 @@
         <v>120</v>
       </c>
       <c r="G1132" s="5" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="H1132" s="6">
         <v>43905</v>
@@ -28867,7 +28882,7 @@
         <v>123</v>
       </c>
       <c r="G1135" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="H1135" s="6">
         <v>43903</v>
@@ -28896,7 +28911,7 @@
         <v>119</v>
       </c>
       <c r="G1136" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H1136" s="6">
         <v>43901</v>
@@ -28925,7 +28940,7 @@
         <v>131</v>
       </c>
       <c r="G1137" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H1137" s="6">
         <v>43903</v>
@@ -28954,7 +28969,7 @@
         <v>125</v>
       </c>
       <c r="G1138" s="5" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="H1138" s="6">
         <v>43906</v>
@@ -29058,7 +29073,7 @@
         <v>119</v>
       </c>
       <c r="G1142" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H1142" s="6">
         <v>43901</v>
@@ -29087,7 +29102,7 @@
         <v>119</v>
       </c>
       <c r="G1143" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H1143" s="6">
         <v>43900</v>
@@ -29116,7 +29131,7 @@
         <v>119</v>
       </c>
       <c r="G1144" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H1144" s="6">
         <v>43904</v>
@@ -29145,7 +29160,7 @@
         <v>119</v>
       </c>
       <c r="G1145" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H1145" s="6">
         <v>43904</v>
@@ -29203,7 +29218,7 @@
         <v>132</v>
       </c>
       <c r="G1147" s="5" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="H1147" s="6">
         <v>43905</v>
@@ -29232,7 +29247,7 @@
         <v>120</v>
       </c>
       <c r="G1148" s="5" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H1148" s="6">
         <v>43898</v>
@@ -29311,7 +29326,7 @@
         <v>120</v>
       </c>
       <c r="G1151" s="5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="H1151" s="6">
         <v>43903</v>
@@ -29365,7 +29380,7 @@
         <v>119</v>
       </c>
       <c r="G1153" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H1153" s="6">
         <v>43895</v>
@@ -29436,7 +29451,7 @@
         <v>131</v>
       </c>
       <c r="G1156" s="5" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="H1156" s="6">
         <v>43886</v>
@@ -29465,7 +29480,7 @@
         <v>131</v>
       </c>
       <c r="G1157" s="5" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="H1157" s="6">
         <v>43886</v>
@@ -29542,7 +29557,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43979.375</v>
+        <v>43980.375</v>
       </c>
       <c r="B2" s="1"/>
     </row>
@@ -31087,7 +31102,7 @@
         <v>120</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H75" s="6">
         <v>43911</v>
@@ -31621,7 +31636,7 @@
         <v>131</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H99" s="6">
         <v>43909</v>
@@ -31650,7 +31665,7 @@
         <v>125</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="H100" s="6">
         <v>43913</v>
@@ -32625,7 +32640,7 @@
       </c>
       <c r="F145" s="5"/>
       <c r="G145" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H145" s="6">
         <v>43906</v>
@@ -34205,7 +34220,7 @@
         <v>120</v>
       </c>
       <c r="G219" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H219" s="6">
         <v>43908</v>
@@ -34656,7 +34671,7 @@
       </c>
       <c r="F240" s="5"/>
       <c r="G240" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H240" s="6">
         <v>43915</v>
@@ -35054,7 +35069,7 @@
       </c>
       <c r="F258" s="5"/>
       <c r="G258" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H258" s="6">
         <v>43912</v>
@@ -35249,7 +35264,7 @@
         <v>119</v>
       </c>
       <c r="G267" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H267" s="6"/>
       <c r="I267" s="6">
@@ -35343,7 +35358,7 @@
         <v>120</v>
       </c>
       <c r="G271" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H271" s="6">
         <v>43911</v>
@@ -35412,7 +35427,7 @@
       </c>
       <c r="F274" s="5"/>
       <c r="G274" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H274" s="6">
         <v>43913</v>
@@ -35675,7 +35690,7 @@
         <v>119</v>
       </c>
       <c r="G285" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H285" s="6">
         <v>43913</v>
@@ -35723,7 +35738,7 @@
       </c>
       <c r="F287" s="5"/>
       <c r="G287" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H287" s="6">
         <v>43907</v>
@@ -35876,7 +35891,7 @@
         <v>120</v>
       </c>
       <c r="G294" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H294" s="6">
         <v>43908</v>
@@ -36052,7 +36067,7 @@
         <v>120</v>
       </c>
       <c r="G302" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H302" s="6">
         <v>43908</v>
@@ -36081,7 +36096,7 @@
         <v>139</v>
       </c>
       <c r="G303" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H303" s="6">
         <v>43909</v>
@@ -36252,7 +36267,7 @@
         <v>120</v>
       </c>
       <c r="G310" s="5" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="H310" s="6">
         <v>43909</v>
@@ -36457,7 +36472,7 @@
         <v>123</v>
       </c>
       <c r="G319" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H319" s="6">
         <v>43908</v>
@@ -36486,7 +36501,7 @@
         <v>123</v>
       </c>
       <c r="G320" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H320" s="6">
         <v>43908</v>
@@ -36565,7 +36580,7 @@
         <v>147</v>
       </c>
       <c r="G323" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H323" s="6">
         <v>43909</v>
@@ -36678,7 +36693,7 @@
         <v>119</v>
       </c>
       <c r="G328" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H328" s="6">
         <v>43909</v>
@@ -36805,7 +36820,7 @@
         <v>119</v>
       </c>
       <c r="G333" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H333" s="6">
         <v>43907</v>
@@ -37286,7 +37301,7 @@
         <v>119</v>
       </c>
       <c r="G354" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H354" s="6">
         <v>43884</v>

</xml_diff>

<commit_message>
updated for the 31st May
</commit_message>
<xml_diff>
--- a/data/NZ_COVID19_data.xlsx
+++ b/data/NZ_COVID19_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\moh.govt.nz\dfs-userdata\userstate\crawson\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\moh.govt.nz\dfs-userdata\UserState\cpollock\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24E47580-291A-4619-84B9-B914FC9E2473}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FA64674-2836-43E5-B907-112913EF0D07}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="25080" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8598" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8597" uniqueCount="336">
   <si>
     <t>NZ526</t>
   </si>
@@ -874,9 +874,6 @@
     <t>MH133</t>
   </si>
   <si>
-    <t>WGN-AKL</t>
-  </si>
-  <si>
     <t>MH145</t>
   </si>
   <si>
@@ -1419,7 +1416,7 @@
   <dimension ref="A1:I1158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="I476" sqref="I476"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,7 +1440,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
-        <v>43981.375</v>
+        <v>43982.375</v>
       </c>
       <c r="B2" s="6"/>
     </row>
@@ -1911,7 +1908,7 @@
         <v>121</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5">
@@ -21763,9 +21760,7 @@
       <c r="F861" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="G861" s="4" t="s">
-        <v>280</v>
-      </c>
+      <c r="G861" s="4"/>
       <c r="H861" s="5"/>
       <c r="I861" s="5">
         <v>43909</v>
@@ -22037,7 +22032,7 @@
         <v>147</v>
       </c>
       <c r="G872" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H872" s="5">
         <v>43905</v>
@@ -22301,7 +22296,7 @@
         <v>120</v>
       </c>
       <c r="G882" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H882" s="5">
         <v>43911</v>
@@ -22330,7 +22325,7 @@
         <v>126</v>
       </c>
       <c r="G883" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H883" s="5">
         <v>43914</v>
@@ -22580,7 +22575,7 @@
         <v>148</v>
       </c>
       <c r="G893" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H893" s="5">
         <v>43906</v>
@@ -22609,7 +22604,7 @@
         <v>148</v>
       </c>
       <c r="G894" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H894" s="5">
         <v>43906</v>
@@ -22686,7 +22681,7 @@
         <v>127</v>
       </c>
       <c r="G897" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H897" s="5">
         <v>43909</v>
@@ -22919,7 +22914,7 @@
         <v>127</v>
       </c>
       <c r="G906" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H906" s="5">
         <v>43909</v>
@@ -22990,7 +22985,7 @@
         <v>150</v>
       </c>
       <c r="G909" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H909" s="5"/>
       <c r="I909" s="5">
@@ -23017,7 +23012,7 @@
         <v>150</v>
       </c>
       <c r="G910" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H910" s="5">
         <v>43909</v>
@@ -23044,7 +23039,7 @@
       </c>
       <c r="F911" s="4"/>
       <c r="G911" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H911" s="5">
         <v>43909</v>
@@ -23326,7 +23321,7 @@
         <v>120</v>
       </c>
       <c r="G923" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H923" s="5">
         <v>43912</v>
@@ -23443,7 +23438,7 @@
         <v>122</v>
       </c>
       <c r="G928" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H928" s="5">
         <v>43901</v>
@@ -23574,7 +23569,7 @@
         <v>120</v>
       </c>
       <c r="G933" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H933" s="5">
         <v>43912</v>
@@ -23703,7 +23698,7 @@
         <v>145</v>
       </c>
       <c r="G938" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H938" s="5">
         <v>43905</v>
@@ -23782,7 +23777,7 @@
         <v>128</v>
       </c>
       <c r="G941" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H941" s="5">
         <v>43903</v>
@@ -23811,7 +23806,7 @@
         <v>120</v>
       </c>
       <c r="G942" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H942" s="5">
         <v>43909</v>
@@ -23898,7 +23893,7 @@
         <v>119</v>
       </c>
       <c r="G945" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H945" s="5">
         <v>43911</v>
@@ -24077,7 +24072,7 @@
         <v>118</v>
       </c>
       <c r="G952" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H952" s="5">
         <v>43910</v>
@@ -24106,7 +24101,7 @@
         <v>141</v>
       </c>
       <c r="G953" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H953" s="5">
         <v>43910</v>
@@ -24297,7 +24292,7 @@
         <v>119</v>
       </c>
       <c r="G960" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H960" s="5">
         <v>43910</v>
@@ -24347,7 +24342,7 @@
         <v>119</v>
       </c>
       <c r="G962" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H962" s="5">
         <v>43910</v>
@@ -24405,7 +24400,7 @@
         <v>120</v>
       </c>
       <c r="G964" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H964" s="5">
         <v>43910</v>
@@ -24434,7 +24429,7 @@
         <v>127</v>
       </c>
       <c r="G965" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H965" s="5">
         <v>43908</v>
@@ -24463,7 +24458,7 @@
         <v>119</v>
       </c>
       <c r="G966" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H966" s="5">
         <v>43910</v>
@@ -24492,7 +24487,7 @@
         <v>119</v>
       </c>
       <c r="G967" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H967" s="5">
         <v>43910</v>
@@ -24685,7 +24680,7 @@
         <v>120</v>
       </c>
       <c r="G974" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H974" s="5"/>
       <c r="I974" s="5">
@@ -24733,7 +24728,7 @@
         <v>132</v>
       </c>
       <c r="G976" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H976" s="5">
         <v>43906</v>
@@ -24870,7 +24865,7 @@
         <v>123</v>
       </c>
       <c r="G981" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H981" s="5">
         <v>43911</v>
@@ -24945,7 +24940,7 @@
         <v>154</v>
       </c>
       <c r="G984" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H984" s="5">
         <v>43909</v>
@@ -25149,7 +25144,7 @@
         <v>119</v>
       </c>
       <c r="G992" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H992" s="5">
         <v>43907</v>
@@ -25299,7 +25294,7 @@
         <v>145</v>
       </c>
       <c r="G998" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H998" s="5">
         <v>43905</v>
@@ -25349,7 +25344,7 @@
         <v>120</v>
       </c>
       <c r="G1000" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H1000" s="5">
         <v>43909</v>
@@ -25407,7 +25402,7 @@
         <v>147</v>
       </c>
       <c r="G1002" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H1002" s="5">
         <v>43905</v>
@@ -25465,7 +25460,7 @@
         <v>131</v>
       </c>
       <c r="G1004" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H1004" s="5">
         <v>43911</v>
@@ -25592,7 +25587,7 @@
         <v>131</v>
       </c>
       <c r="G1009" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H1009" s="5">
         <v>43909</v>
@@ -25650,7 +25645,7 @@
         <v>119</v>
       </c>
       <c r="G1011" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H1011" s="5">
         <v>43909</v>
@@ -25735,7 +25730,7 @@
         <v>119</v>
       </c>
       <c r="G1014" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H1014" s="5">
         <v>43909</v>
@@ -25849,7 +25844,7 @@
         <v>120</v>
       </c>
       <c r="G1018" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H1018" s="5">
         <v>43907</v>
@@ -25878,7 +25873,7 @@
         <v>120</v>
       </c>
       <c r="G1019" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H1019" s="5">
         <v>43903</v>
@@ -25936,7 +25931,7 @@
         <v>127</v>
       </c>
       <c r="G1021" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H1021" s="5">
         <v>43907</v>
@@ -25986,7 +25981,7 @@
         <v>120</v>
       </c>
       <c r="G1023" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H1023" s="5">
         <v>43908</v>
@@ -26132,7 +26127,7 @@
         <v>125</v>
       </c>
       <c r="G1029" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H1029" s="5">
         <v>43909</v>
@@ -26525,7 +26520,7 @@
         <v>131</v>
       </c>
       <c r="G1044" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H1044" s="5">
         <v>43907</v>
@@ -26654,7 +26649,7 @@
         <v>119</v>
       </c>
       <c r="G1049" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H1049" s="5">
         <v>43906</v>
@@ -26866,7 +26861,7 @@
         <v>119</v>
       </c>
       <c r="G1057" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H1057" s="5">
         <v>43906</v>
@@ -26922,7 +26917,7 @@
       </c>
       <c r="F1059" s="4"/>
       <c r="G1059" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H1059" s="5">
         <v>43898</v>
@@ -26970,7 +26965,7 @@
         <v>120</v>
       </c>
       <c r="G1061" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H1061" s="5"/>
       <c r="I1061" s="5">
@@ -26997,7 +26992,7 @@
         <v>146</v>
       </c>
       <c r="G1062" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H1062" s="5">
         <v>43910</v>
@@ -27026,7 +27021,7 @@
         <v>120</v>
       </c>
       <c r="G1063" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H1063" s="5">
         <v>43908</v>
@@ -27055,7 +27050,7 @@
         <v>120</v>
       </c>
       <c r="G1064" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H1064" s="5"/>
       <c r="I1064" s="5">
@@ -27082,7 +27077,7 @@
         <v>120</v>
       </c>
       <c r="G1065" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H1065" s="5">
         <v>43905</v>
@@ -27344,7 +27339,7 @@
       </c>
       <c r="F1075" s="4"/>
       <c r="G1075" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H1075" s="5">
         <v>43907</v>
@@ -27369,7 +27364,7 @@
       </c>
       <c r="F1076" s="4"/>
       <c r="G1076" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H1076" s="5">
         <v>43905</v>
@@ -27521,7 +27516,7 @@
         <v>146</v>
       </c>
       <c r="G1082" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H1082" s="5">
         <v>43908</v>
@@ -27894,7 +27889,7 @@
         <v>123</v>
       </c>
       <c r="G1097" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H1097" s="5">
         <v>43907</v>
@@ -27971,7 +27966,7 @@
       </c>
       <c r="F1100" s="4"/>
       <c r="G1100" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H1100" s="5">
         <v>43905</v>
@@ -28027,7 +28022,7 @@
         <v>123</v>
       </c>
       <c r="G1102" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H1102" s="5">
         <v>43907</v>
@@ -28085,7 +28080,7 @@
         <v>119</v>
       </c>
       <c r="G1104" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H1104" s="5">
         <v>43906</v>
@@ -28436,7 +28431,7 @@
         <v>120</v>
       </c>
       <c r="G1117" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H1117" s="5">
         <v>43904</v>
@@ -28465,7 +28460,7 @@
         <v>119</v>
       </c>
       <c r="G1118" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H1118" s="5"/>
       <c r="I1118" s="5">
@@ -28540,7 +28535,7 @@
       </c>
       <c r="F1121" s="4"/>
       <c r="G1121" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H1121" s="5">
         <v>43903</v>
@@ -28698,7 +28693,7 @@
       </c>
       <c r="F1127" s="4"/>
       <c r="G1127" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H1127" s="5">
         <v>43894</v>
@@ -28831,7 +28826,7 @@
         <v>120</v>
       </c>
       <c r="G1132" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H1132" s="5">
         <v>43905</v>
@@ -28914,7 +28909,7 @@
         <v>123</v>
       </c>
       <c r="G1135" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H1135" s="5">
         <v>43903</v>
@@ -29001,7 +28996,7 @@
         <v>125</v>
       </c>
       <c r="G1138" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H1138" s="5">
         <v>43906</v>
@@ -29250,7 +29245,7 @@
         <v>132</v>
       </c>
       <c r="G1147" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H1147" s="5">
         <v>43905</v>
@@ -29279,7 +29274,7 @@
         <v>120</v>
       </c>
       <c r="G1148" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H1148" s="5">
         <v>43898</v>
@@ -29358,7 +29353,7 @@
         <v>120</v>
       </c>
       <c r="G1151" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H1151" s="5">
         <v>43903</v>
@@ -29483,7 +29478,7 @@
         <v>131</v>
       </c>
       <c r="G1156" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H1156" s="5">
         <v>43886</v>
@@ -29512,7 +29507,7 @@
         <v>131</v>
       </c>
       <c r="G1157" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H1157" s="5">
         <v>43886</v>
@@ -29566,7 +29561,7 @@
   </sheetPr>
   <dimension ref="A1:I354"/>
   <sheetViews>
-    <sheetView topLeftCell="A346" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -29589,7 +29584,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
-        <v>43981.375</v>
+        <v>43982.375</v>
       </c>
       <c r="B2" s="6"/>
     </row>
@@ -36303,7 +36298,7 @@
         <v>120</v>
       </c>
       <c r="G310" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H310" s="5">
         <v>43909</v>
@@ -37212,7 +37207,7 @@
         <v>127</v>
       </c>
       <c r="G349" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H349" s="5">
         <v>43905</v>
@@ -37353,231 +37348,4 @@
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup paperSize="9" scale="43" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003ABA77D7CF804044887C9E6FB5E413B1" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8238a55b249c6a1da64af20f08a2bf62">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="912cedb3-7f04-47c0-a283-ea387d34e08f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="776a5dbc1ed470d08fc62ab88000e5e1" ns3:_="">
-    <xsd:import namespace="912cedb3-7f04-47c0-a283-ea387d34e08f"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="912cedb3-7f04-47c0-a283-ea387d34e08f" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B41F072F-FC2B-4767-A85F-7840EDC50193}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="912cedb3-7f04-47c0-a283-ea387d34e08f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83AF193-C9B5-40E2-B176-4A8D71929EF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F8A80C4-7A1A-4676-8964-04F742CCFC46}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="912cedb3-7f04-47c0-a283-ea387d34e08f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>